<commit_message>
FIn modale explicative, fix bug download example template
</commit_message>
<xml_diff>
--- a/public/fichiers/template_import.xlsx
+++ b/public/fichiers/template_import.xlsx
@@ -1671,9 +1671,6 @@
     <t>Nb</t>
   </si>
   <si>
-    <t xml:space="preserve">LISTE DES loisirs 2022 / 2023 </t>
-  </si>
-  <si>
     <t>Classement</t>
   </si>
   <si>
@@ -1708,6 +1705,9 @@
   </si>
   <si>
     <t>Licence</t>
+  </si>
+  <si>
+    <t>LISTE DES JOUEURS - ESFTT</t>
   </si>
 </sst>
 </file>
@@ -5672,7 +5672,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="74" zoomScalePageLayoutView="55" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
+      <selection pane="bottomLeft" sqref="A1:J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="22.8"/>
@@ -5699,7 +5699,7 @@
   <sheetData>
     <row r="1" spans="1:17" ht="39" customHeight="1" thickBot="1">
       <c r="A1" s="257" t="s">
-        <v>550</v>
+        <v>562</v>
       </c>
       <c r="B1" s="258"/>
       <c r="C1" s="258"/>
@@ -5730,7 +5730,7 @@
         <v>549</v>
       </c>
       <c r="B3" s="226" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="C3" s="234" t="s">
         <v>132</v>
@@ -5739,43 +5739,43 @@
         <v>133</v>
       </c>
       <c r="E3" s="222" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="F3" s="222" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="G3" s="222" t="s">
         <v>135</v>
       </c>
       <c r="H3" s="222" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="I3" s="222" t="s">
         <v>136</v>
       </c>
       <c r="J3" s="222" t="s">
+        <v>557</v>
+      </c>
+      <c r="K3" s="222" t="s">
+        <v>550</v>
+      </c>
+      <c r="L3" s="222" t="s">
+        <v>551</v>
+      </c>
+      <c r="M3" s="222" t="s">
         <v>558</v>
       </c>
-      <c r="K3" s="222" t="s">
-        <v>551</v>
-      </c>
-      <c r="L3" s="222" t="s">
+      <c r="N3" s="222" t="s">
         <v>552</v>
       </c>
-      <c r="M3" s="222" t="s">
-        <v>559</v>
-      </c>
-      <c r="N3" s="222" t="s">
+      <c r="O3" s="222" t="s">
         <v>553</v>
       </c>
-      <c r="O3" s="222" t="s">
+      <c r="P3" s="222" t="s">
+        <v>555</v>
+      </c>
+      <c r="Q3" s="222" t="s">
         <v>554</v>
-      </c>
-      <c r="P3" s="222" t="s">
-        <v>556</v>
-      </c>
-      <c r="Q3" s="222" t="s">
-        <v>555</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="40.049999999999997" customHeight="1">

</xml_diff>

<commit_message>
Catégorie Jeune, roles errors plus précis, style nb matches joués, remove custom selected players icon cursor pointer
</commit_message>
<xml_diff>
--- a/public/fichiers/template_import.xlsx
+++ b/public/fichiers/template_import.xlsx
@@ -15,11 +15,12 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Fichier Maître Saison 17-18 '!$A$1:$J$26</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="869" uniqueCount="563">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="870" uniqueCount="564">
   <si>
     <t>Patrick</t>
   </si>
@@ -1708,6 +1709,9 @@
   </si>
   <si>
     <t>LISTE DES JOUEURS - ESFTT</t>
+  </si>
+  <si>
+    <t>Jeune</t>
   </si>
 </sst>
 </file>
@@ -1717,7 +1721,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="myy\i\l"/>
   </numFmts>
-  <fonts count="36">
+  <fonts count="38">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1956,6 +1960,19 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="12">
     <fill>
@@ -2025,7 +2042,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="38">
+  <borders count="43">
     <border>
       <left/>
       <right/>
@@ -2488,6 +2505,63 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1055">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -3546,7 +3620,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="262">
+  <cellXfs count="257">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4179,15 +4253,10 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="9" borderId="37" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="9" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -4195,12 +4264,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="35" fillId="9" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="9" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -4210,90 +4273,76 @@
     <xf numFmtId="49" fontId="7" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="9" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="13" fillId="9" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="9" borderId="37" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="35" fillId="9" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="9" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="9" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="4" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="34" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="33" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="34" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="33" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="33" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="4" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="13" fillId="9" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="33" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="33" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="9" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="34" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="34" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="34" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="34" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="34" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="33" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="33" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="33" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4301,6 +4350,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="37" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="36" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -5668,559 +5729,3592 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Q27"/>
+  <dimension ref="A1:R358"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="74" zoomScalePageLayoutView="55" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:J1"/>
+    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" zoomScalePageLayoutView="55" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A319" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R326" sqref="R326"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="22.8"/>
   <cols>
-    <col min="1" max="1" width="7.109375" style="256" customWidth="1"/>
-    <col min="2" max="2" width="25.44140625" style="250" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.33203125" style="219" customWidth="1"/>
-    <col min="4" max="4" width="20.21875" style="219" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="32.6640625" style="219" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.33203125" style="219" customWidth="1"/>
-    <col min="7" max="7" width="21.6640625" style="220" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.21875" style="224" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="65.109375" style="224" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="50.77734375" style="225" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.21875" style="220" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.88671875" style="220" customWidth="1"/>
-    <col min="13" max="13" width="17.21875" style="220" customWidth="1"/>
-    <col min="14" max="14" width="22.33203125" style="220" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="29.88671875" style="220" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19.5546875" style="220" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="26.77734375" style="220" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="7.109375" style="246" customWidth="1"/>
+    <col min="2" max="2" width="25.44140625" style="227" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.33203125" style="218" customWidth="1"/>
+    <col min="4" max="4" width="20.21875" style="218" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.6640625" style="218" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.33203125" style="218" customWidth="1"/>
+    <col min="7" max="7" width="21.6640625" style="219" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.21875" style="221" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="65.109375" style="221" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="50.77734375" style="222" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.21875" style="219" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.21875" style="219" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11" style="219" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.6640625" style="219" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.6640625" style="219" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="29.5546875" style="219" customWidth="1"/>
+    <col min="17" max="17" width="19" style="219" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="26" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="39" customHeight="1" thickBot="1">
-      <c r="A1" s="257" t="s">
+    <row r="1" spans="1:18" ht="39" customHeight="1" thickBot="1">
+      <c r="A1" s="247" t="s">
         <v>562</v>
       </c>
-      <c r="B1" s="258"/>
-      <c r="C1" s="258"/>
-      <c r="D1" s="258"/>
-      <c r="E1" s="258"/>
-      <c r="F1" s="258"/>
-      <c r="G1" s="258"/>
-      <c r="H1" s="258"/>
-      <c r="I1" s="258"/>
-      <c r="J1" s="258"/>
-      <c r="K1" s="219"/>
-    </row>
-    <row r="2" spans="1:17" ht="17.25" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A2" s="233"/>
-      <c r="B2" s="227"/>
-      <c r="C2" s="232"/>
-      <c r="D2" s="232"/>
-      <c r="E2" s="232"/>
-      <c r="F2" s="232"/>
-      <c r="G2" s="221"/>
-      <c r="H2" s="221"/>
-      <c r="I2" s="221"/>
-      <c r="J2" s="221"/>
-      <c r="K2" s="221"/>
-    </row>
-    <row r="3" spans="1:17" ht="100.95" customHeight="1" thickBot="1">
-      <c r="A3" s="241" t="s">
+      <c r="B1" s="248"/>
+      <c r="C1" s="248"/>
+      <c r="D1" s="248"/>
+      <c r="E1" s="248"/>
+      <c r="F1" s="248"/>
+      <c r="G1" s="248"/>
+      <c r="H1" s="248"/>
+      <c r="I1" s="248"/>
+      <c r="J1" s="248"/>
+      <c r="K1" s="248"/>
+      <c r="L1" s="248"/>
+      <c r="M1" s="248"/>
+      <c r="N1" s="248"/>
+      <c r="O1" s="248"/>
+      <c r="P1" s="248"/>
+      <c r="Q1" s="248"/>
+      <c r="R1" s="248"/>
+    </row>
+    <row r="2" spans="1:18" ht="17.25" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A2" s="249"/>
+      <c r="B2" s="249"/>
+      <c r="C2" s="249"/>
+      <c r="D2" s="249"/>
+      <c r="E2" s="249"/>
+      <c r="F2" s="249"/>
+      <c r="G2" s="249"/>
+      <c r="H2" s="249"/>
+      <c r="I2" s="249"/>
+      <c r="J2" s="249"/>
+      <c r="K2" s="249"/>
+      <c r="L2" s="249"/>
+      <c r="M2" s="249"/>
+      <c r="N2" s="249"/>
+      <c r="O2" s="249"/>
+      <c r="P2" s="249"/>
+      <c r="Q2" s="249"/>
+      <c r="R2" s="249"/>
+    </row>
+    <row r="3" spans="1:18" s="239" customFormat="1" ht="100.95" customHeight="1" thickBot="1">
+      <c r="A3" s="226" t="s">
         <v>549</v>
       </c>
-      <c r="B3" s="226" t="s">
+      <c r="B3" s="231" t="s">
         <v>561</v>
       </c>
-      <c r="C3" s="234" t="s">
+      <c r="C3" s="232" t="s">
         <v>132</v>
       </c>
-      <c r="D3" s="231" t="s">
+      <c r="D3" s="233" t="s">
         <v>133</v>
       </c>
-      <c r="E3" s="222" t="s">
+      <c r="E3" s="234" t="s">
         <v>560</v>
       </c>
-      <c r="F3" s="222" t="s">
+      <c r="F3" s="234" t="s">
         <v>559</v>
       </c>
-      <c r="G3" s="222" t="s">
+      <c r="G3" s="234" t="s">
         <v>135</v>
       </c>
-      <c r="H3" s="222" t="s">
+      <c r="H3" s="234" t="s">
         <v>556</v>
       </c>
-      <c r="I3" s="222" t="s">
+      <c r="I3" s="234" t="s">
         <v>136</v>
       </c>
-      <c r="J3" s="222" t="s">
+      <c r="J3" s="234" t="s">
         <v>557</v>
       </c>
-      <c r="K3" s="222" t="s">
+      <c r="K3" s="234" t="s">
         <v>550</v>
       </c>
-      <c r="L3" s="222" t="s">
+      <c r="L3" s="234" t="s">
         <v>551</v>
       </c>
-      <c r="M3" s="222" t="s">
+      <c r="M3" s="234" t="s">
+        <v>563</v>
+      </c>
+      <c r="N3" s="234" t="s">
         <v>558</v>
       </c>
-      <c r="N3" s="222" t="s">
+      <c r="O3" s="234" t="s">
         <v>552</v>
       </c>
-      <c r="O3" s="222" t="s">
+      <c r="P3" s="234" t="s">
         <v>553</v>
       </c>
-      <c r="P3" s="222" t="s">
+      <c r="Q3" s="234" t="s">
         <v>555</v>
       </c>
-      <c r="Q3" s="222" t="s">
+      <c r="R3" s="245" t="s">
         <v>554</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="40.049999999999997" customHeight="1">
-      <c r="A4" s="240"/>
-      <c r="B4" s="240"/>
-      <c r="C4" s="239"/>
-      <c r="D4" s="243"/>
-      <c r="E4" s="252"/>
-      <c r="F4" s="252"/>
-      <c r="G4" s="252"/>
-      <c r="H4" s="252"/>
+    <row r="4" spans="1:18" s="239" customFormat="1" ht="40.049999999999997" customHeight="1">
+      <c r="A4" s="229"/>
+      <c r="B4" s="235"/>
+      <c r="C4" s="236"/>
+      <c r="D4" s="236"/>
+      <c r="E4" s="236"/>
+      <c r="F4" s="236"/>
+      <c r="G4" s="236"/>
+      <c r="H4" s="236"/>
       <c r="I4" s="237"/>
-      <c r="J4" s="251"/>
-      <c r="K4" s="250"/>
-      <c r="L4" s="250"/>
-      <c r="M4" s="250"/>
-      <c r="N4" s="250"/>
-      <c r="O4" s="250"/>
-      <c r="P4" s="250"/>
-      <c r="Q4" s="250"/>
-    </row>
-    <row r="5" spans="1:17" ht="40.049999999999997" customHeight="1">
-      <c r="A5" s="239"/>
-      <c r="C5" s="239"/>
-      <c r="D5" s="243"/>
-      <c r="E5" s="252"/>
-      <c r="F5" s="252"/>
-      <c r="G5" s="252"/>
-      <c r="H5" s="252"/>
-      <c r="I5" s="254"/>
-      <c r="J5" s="254"/>
-      <c r="K5" s="250"/>
-      <c r="L5" s="250"/>
-      <c r="M5" s="250"/>
-      <c r="N5" s="250"/>
-      <c r="O5" s="250"/>
-      <c r="P5" s="250"/>
-      <c r="Q5" s="250"/>
-    </row>
-    <row r="6" spans="1:17" ht="40.049999999999997" customHeight="1">
-      <c r="A6" s="239"/>
-      <c r="B6" s="239"/>
-      <c r="C6" s="239"/>
-      <c r="D6" s="243"/>
-      <c r="E6" s="252"/>
-      <c r="F6" s="243"/>
-      <c r="G6" s="238"/>
-      <c r="H6" s="252"/>
-      <c r="I6" s="254"/>
-      <c r="J6" s="249"/>
-      <c r="K6" s="250"/>
-      <c r="L6" s="250"/>
-      <c r="M6" s="250"/>
-      <c r="N6" s="250"/>
-      <c r="O6" s="250"/>
-      <c r="P6" s="250"/>
-      <c r="Q6" s="250"/>
-    </row>
-    <row r="7" spans="1:17" ht="40.049999999999997" customHeight="1">
-      <c r="A7" s="239"/>
-      <c r="B7" s="239"/>
-      <c r="C7" s="239"/>
-      <c r="D7" s="243"/>
-      <c r="G7" s="252"/>
-      <c r="H7" s="252"/>
-      <c r="I7" s="236"/>
-      <c r="J7" s="249"/>
-      <c r="K7" s="250"/>
-      <c r="L7" s="250"/>
-      <c r="M7" s="250"/>
-      <c r="N7" s="250"/>
-      <c r="O7" s="250"/>
-      <c r="P7" s="250"/>
-      <c r="Q7" s="250"/>
-    </row>
-    <row r="8" spans="1:17" ht="40.049999999999997" customHeight="1">
-      <c r="A8" s="239"/>
-      <c r="B8" s="239"/>
-      <c r="C8" s="239"/>
-      <c r="D8" s="243"/>
-      <c r="E8" s="252"/>
-      <c r="F8" s="252"/>
-      <c r="G8" s="252"/>
-      <c r="H8" s="252"/>
-      <c r="I8" s="235"/>
-      <c r="J8" s="248"/>
-      <c r="K8" s="250"/>
-      <c r="L8" s="250"/>
-      <c r="M8" s="250"/>
-      <c r="N8" s="250"/>
-      <c r="O8" s="250"/>
-      <c r="P8" s="250"/>
-      <c r="Q8" s="250"/>
-    </row>
-    <row r="9" spans="1:17" ht="40.049999999999997" customHeight="1">
-      <c r="A9" s="239"/>
-      <c r="B9" s="239"/>
-      <c r="C9" s="239"/>
-      <c r="D9" s="243"/>
-      <c r="E9" s="252"/>
-      <c r="F9" s="252"/>
-      <c r="G9" s="252"/>
-      <c r="H9" s="252"/>
-      <c r="I9" s="236"/>
-      <c r="J9" s="249"/>
-      <c r="K9" s="250"/>
-      <c r="L9" s="250"/>
-      <c r="M9" s="250"/>
-      <c r="N9" s="250"/>
-      <c r="O9" s="250"/>
-      <c r="P9" s="250"/>
-      <c r="Q9" s="250"/>
-    </row>
-    <row r="10" spans="1:17" ht="40.049999999999997" customHeight="1">
-      <c r="A10" s="240"/>
-      <c r="B10" s="240"/>
-      <c r="C10" s="239"/>
-      <c r="D10" s="243"/>
-      <c r="E10" s="252"/>
-      <c r="F10" s="252"/>
-      <c r="G10" s="252"/>
-      <c r="H10" s="252"/>
-      <c r="I10" s="254"/>
-      <c r="J10" s="249"/>
-      <c r="K10" s="250"/>
-      <c r="L10" s="250"/>
-      <c r="M10" s="250"/>
-      <c r="N10" s="250"/>
-      <c r="O10" s="250"/>
-      <c r="P10" s="250"/>
-      <c r="Q10" s="250"/>
-    </row>
-    <row r="11" spans="1:17" ht="40.049999999999997" customHeight="1">
-      <c r="A11" s="240"/>
-      <c r="B11" s="240"/>
-      <c r="C11" s="239"/>
-      <c r="D11" s="243"/>
-      <c r="E11" s="252"/>
-      <c r="F11" s="252"/>
-      <c r="G11" s="252"/>
-      <c r="H11" s="252"/>
-      <c r="I11" s="254"/>
-      <c r="J11" s="251"/>
-      <c r="K11" s="250"/>
-      <c r="L11" s="250"/>
-      <c r="M11" s="250"/>
-      <c r="N11" s="250"/>
-      <c r="O11" s="250"/>
-      <c r="P11" s="250"/>
-      <c r="Q11" s="250"/>
-    </row>
-    <row r="12" spans="1:17" ht="40.049999999999997" customHeight="1">
-      <c r="A12" s="239"/>
-      <c r="B12" s="239"/>
-      <c r="C12" s="239"/>
-      <c r="D12" s="243"/>
-      <c r="E12" s="252"/>
-      <c r="F12" s="252"/>
-      <c r="G12" s="252"/>
-      <c r="H12" s="250"/>
-      <c r="I12" s="254"/>
-      <c r="J12" s="251"/>
-      <c r="K12" s="250"/>
-      <c r="L12" s="250"/>
-      <c r="M12" s="250"/>
-      <c r="N12" s="250"/>
-      <c r="O12" s="250"/>
-      <c r="P12" s="250"/>
-      <c r="Q12" s="250"/>
-    </row>
-    <row r="13" spans="1:17" ht="40.049999999999997" customHeight="1">
-      <c r="A13" s="239"/>
-      <c r="B13" s="239"/>
-      <c r="C13" s="239"/>
-      <c r="D13" s="243"/>
-      <c r="E13" s="252"/>
-      <c r="F13" s="252"/>
-      <c r="G13" s="252"/>
-      <c r="H13" s="252"/>
-      <c r="I13" s="254"/>
-      <c r="J13" s="249"/>
-      <c r="K13" s="250"/>
-      <c r="L13" s="250"/>
-      <c r="M13" s="250"/>
-      <c r="N13" s="250"/>
-      <c r="O13" s="250"/>
-      <c r="P13" s="250"/>
-      <c r="Q13" s="250"/>
-    </row>
-    <row r="14" spans="1:17" ht="40.049999999999997" customHeight="1">
-      <c r="A14" s="239"/>
-      <c r="B14" s="239"/>
-      <c r="C14" s="239"/>
-      <c r="D14" s="243"/>
-      <c r="E14" s="252"/>
-      <c r="F14" s="252"/>
-      <c r="G14" s="247"/>
-      <c r="H14" s="247"/>
-      <c r="I14" s="255"/>
-      <c r="J14" s="246"/>
-      <c r="K14" s="250"/>
-      <c r="L14" s="250"/>
-      <c r="M14" s="250"/>
-      <c r="N14" s="250"/>
-      <c r="O14" s="250"/>
-      <c r="P14" s="250"/>
-      <c r="Q14" s="250"/>
-    </row>
-    <row r="15" spans="1:17" ht="40.049999999999997" customHeight="1">
-      <c r="A15" s="240"/>
-      <c r="B15" s="240"/>
-      <c r="C15" s="239"/>
-      <c r="D15" s="243"/>
-      <c r="E15" s="252"/>
-      <c r="F15" s="252"/>
-      <c r="G15" s="252"/>
-      <c r="H15" s="252"/>
-      <c r="I15" s="254"/>
-      <c r="J15" s="249"/>
-      <c r="K15" s="250"/>
-      <c r="L15" s="250"/>
-      <c r="M15" s="250"/>
-      <c r="N15" s="250"/>
-      <c r="O15" s="250"/>
-      <c r="P15" s="250"/>
-      <c r="Q15" s="250"/>
-    </row>
-    <row r="16" spans="1:17" ht="40.049999999999997" customHeight="1">
-      <c r="A16" s="240"/>
-      <c r="B16" s="240"/>
-      <c r="C16" s="239"/>
-      <c r="D16" s="243"/>
-      <c r="E16" s="252"/>
-      <c r="F16" s="252"/>
-      <c r="G16" s="245"/>
-      <c r="H16" s="245"/>
-      <c r="I16" s="254"/>
-      <c r="J16" s="249"/>
-      <c r="K16" s="250"/>
-      <c r="L16" s="250"/>
-      <c r="M16" s="250"/>
-      <c r="N16" s="250"/>
-      <c r="O16" s="250"/>
-      <c r="P16" s="250"/>
-      <c r="Q16" s="250"/>
-    </row>
-    <row r="17" spans="1:17" ht="40.049999999999997" customHeight="1">
-      <c r="A17" s="240"/>
-      <c r="B17" s="240"/>
-      <c r="C17" s="239"/>
-      <c r="D17" s="243"/>
-      <c r="E17" s="252"/>
-      <c r="F17" s="252"/>
-      <c r="G17" s="252"/>
-      <c r="H17" s="252"/>
-      <c r="I17" s="254"/>
-      <c r="J17" s="249"/>
-      <c r="K17" s="250"/>
-      <c r="L17" s="250"/>
-      <c r="M17" s="250"/>
-      <c r="N17" s="250"/>
-      <c r="O17" s="250"/>
-      <c r="P17" s="250"/>
-      <c r="Q17" s="250"/>
-    </row>
-    <row r="18" spans="1:17" ht="40.049999999999997" customHeight="1">
-      <c r="A18" s="239"/>
-      <c r="B18" s="239"/>
-      <c r="C18" s="239"/>
-      <c r="D18" s="243"/>
-      <c r="E18" s="252"/>
-      <c r="F18" s="252"/>
-      <c r="G18" s="252"/>
-      <c r="H18" s="244"/>
-      <c r="I18" s="253"/>
-      <c r="J18" s="254"/>
-      <c r="K18" s="250"/>
-      <c r="L18" s="250"/>
-      <c r="M18" s="250"/>
-      <c r="N18" s="250"/>
-      <c r="O18" s="250"/>
-      <c r="P18" s="250"/>
-      <c r="Q18" s="250"/>
-    </row>
-    <row r="19" spans="1:17" ht="40.049999999999997" customHeight="1">
-      <c r="A19" s="240"/>
-      <c r="B19" s="240"/>
-      <c r="C19" s="239"/>
-      <c r="D19" s="243"/>
-      <c r="E19" s="243"/>
-      <c r="F19" s="243"/>
-      <c r="G19" s="244"/>
-      <c r="H19" s="244"/>
-      <c r="I19" s="254"/>
-      <c r="J19" s="249"/>
-      <c r="K19" s="250"/>
-      <c r="L19" s="250"/>
-      <c r="M19" s="250"/>
-      <c r="N19" s="250"/>
-      <c r="O19" s="250"/>
-      <c r="P19" s="250"/>
-      <c r="Q19" s="250"/>
-    </row>
-    <row r="20" spans="1:17" ht="40.049999999999997" customHeight="1">
-      <c r="A20" s="240"/>
-      <c r="B20" s="240"/>
-      <c r="C20" s="239"/>
-      <c r="D20" s="243"/>
-      <c r="G20" s="252"/>
-      <c r="H20" s="252"/>
-      <c r="I20" s="254"/>
-      <c r="J20" s="249"/>
-      <c r="K20" s="250"/>
-      <c r="L20" s="250"/>
-      <c r="M20" s="250"/>
-      <c r="N20" s="250"/>
-      <c r="O20" s="250"/>
-      <c r="P20" s="250"/>
-      <c r="Q20" s="250"/>
-    </row>
-    <row r="21" spans="1:17" ht="40.049999999999997" customHeight="1">
-      <c r="A21" s="240"/>
-      <c r="B21" s="240"/>
-      <c r="C21" s="239"/>
-      <c r="D21" s="243"/>
-      <c r="E21" s="252"/>
-      <c r="F21" s="252"/>
-      <c r="G21" s="252"/>
-      <c r="H21" s="252"/>
-      <c r="I21" s="254"/>
-      <c r="J21" s="249"/>
-      <c r="K21" s="250"/>
-      <c r="L21" s="250"/>
-      <c r="M21" s="250"/>
-      <c r="N21" s="250"/>
-      <c r="O21" s="250"/>
-      <c r="P21" s="250"/>
-      <c r="Q21" s="250"/>
-    </row>
-    <row r="22" spans="1:17" ht="40.049999999999997" customHeight="1">
-      <c r="A22" s="240"/>
-      <c r="B22" s="240"/>
-      <c r="C22" s="239"/>
-      <c r="D22" s="243"/>
-      <c r="E22" s="252"/>
-      <c r="F22" s="252"/>
-      <c r="G22" s="252"/>
-      <c r="H22" s="252"/>
-      <c r="I22" s="254"/>
-      <c r="J22" s="249"/>
-      <c r="K22" s="250"/>
-      <c r="L22" s="250"/>
-      <c r="M22" s="250"/>
-      <c r="N22" s="250"/>
-      <c r="O22" s="250"/>
-      <c r="P22" s="250"/>
-      <c r="Q22" s="250"/>
-    </row>
-    <row r="23" spans="1:17" ht="40.049999999999997" customHeight="1">
-      <c r="A23" s="240"/>
-      <c r="B23" s="240"/>
-      <c r="C23" s="239"/>
-      <c r="D23" s="243"/>
-      <c r="E23" s="252"/>
-      <c r="F23" s="252"/>
-      <c r="G23" s="252"/>
-      <c r="H23" s="252"/>
-      <c r="I23" s="254"/>
-      <c r="J23" s="249"/>
-      <c r="K23" s="250"/>
-      <c r="L23" s="250"/>
-      <c r="M23" s="250"/>
-      <c r="N23" s="250"/>
-      <c r="O23" s="250"/>
-      <c r="P23" s="250"/>
-      <c r="Q23" s="250"/>
-    </row>
-    <row r="24" spans="1:17" ht="40.049999999999997" customHeight="1">
-      <c r="A24" s="240"/>
-      <c r="B24" s="240"/>
-      <c r="C24" s="239"/>
-      <c r="D24" s="243"/>
-      <c r="E24" s="252"/>
-      <c r="F24" s="252"/>
-      <c r="G24" s="252"/>
-      <c r="H24" s="252"/>
-      <c r="I24" s="254"/>
-      <c r="J24" s="249"/>
-      <c r="K24" s="250"/>
-      <c r="L24" s="250"/>
-      <c r="M24" s="250"/>
-      <c r="N24" s="250"/>
-      <c r="O24" s="250"/>
-      <c r="P24" s="250"/>
-      <c r="Q24" s="250"/>
-    </row>
-    <row r="25" spans="1:17" ht="40.049999999999997" customHeight="1">
-      <c r="A25" s="240"/>
-      <c r="B25" s="240"/>
-      <c r="C25" s="239"/>
-      <c r="D25" s="243"/>
-      <c r="E25" s="252"/>
-      <c r="F25" s="252"/>
-      <c r="G25" s="252"/>
-      <c r="H25" s="252"/>
-      <c r="I25" s="254"/>
-      <c r="J25" s="249"/>
-      <c r="K25" s="250"/>
-      <c r="L25" s="250"/>
-      <c r="M25" s="250"/>
-      <c r="N25" s="250"/>
-      <c r="O25" s="250"/>
-      <c r="P25" s="250"/>
-      <c r="Q25" s="250"/>
-    </row>
-    <row r="26" spans="1:17" s="218" customFormat="1" ht="40.049999999999997" customHeight="1">
-      <c r="A26" s="244"/>
-      <c r="B26" s="244"/>
-      <c r="C26" s="244"/>
-      <c r="D26" s="244"/>
-      <c r="E26" s="244"/>
-      <c r="F26" s="244"/>
-      <c r="G26" s="244"/>
-      <c r="H26" s="244"/>
-      <c r="I26" s="236"/>
-      <c r="J26" s="248"/>
-      <c r="K26" s="250"/>
-      <c r="L26" s="242"/>
-      <c r="M26" s="242"/>
-      <c r="N26" s="242"/>
-      <c r="O26" s="242"/>
-      <c r="P26" s="242"/>
-      <c r="Q26" s="242"/>
-    </row>
-    <row r="27" spans="1:17" ht="25.2">
-      <c r="C27" s="230"/>
-      <c r="D27" s="229"/>
-      <c r="E27" s="228"/>
-      <c r="F27" s="228"/>
-      <c r="G27" s="223"/>
+      <c r="J4" s="238"/>
+      <c r="K4" s="228"/>
+      <c r="L4" s="253"/>
+      <c r="M4" s="253"/>
+      <c r="N4" s="253"/>
+      <c r="O4" s="253"/>
+      <c r="P4" s="253"/>
+      <c r="Q4" s="253"/>
+      <c r="R4" s="254"/>
+    </row>
+    <row r="5" spans="1:18" s="239" customFormat="1" ht="40.049999999999997" customHeight="1">
+      <c r="A5" s="230"/>
+      <c r="B5" s="228"/>
+      <c r="C5" s="236"/>
+      <c r="D5" s="236"/>
+      <c r="E5" s="236"/>
+      <c r="F5" s="236"/>
+      <c r="G5" s="236"/>
+      <c r="H5" s="236"/>
+      <c r="I5" s="240"/>
+      <c r="J5" s="240"/>
+      <c r="K5" s="228"/>
+      <c r="L5" s="253"/>
+      <c r="M5" s="253"/>
+      <c r="N5" s="253"/>
+      <c r="O5" s="253"/>
+      <c r="P5" s="253"/>
+      <c r="Q5" s="253"/>
+      <c r="R5" s="254"/>
+    </row>
+    <row r="6" spans="1:18" s="239" customFormat="1" ht="40.049999999999997" customHeight="1">
+      <c r="A6" s="230"/>
+      <c r="B6" s="236"/>
+      <c r="C6" s="236"/>
+      <c r="D6" s="236"/>
+      <c r="E6" s="236"/>
+      <c r="F6" s="236"/>
+      <c r="G6" s="236"/>
+      <c r="H6" s="236"/>
+      <c r="I6" s="240"/>
+      <c r="J6" s="241"/>
+      <c r="K6" s="228"/>
+      <c r="L6" s="253"/>
+      <c r="M6" s="253"/>
+      <c r="N6" s="253"/>
+      <c r="O6" s="253"/>
+      <c r="P6" s="253"/>
+      <c r="Q6" s="253"/>
+      <c r="R6" s="254"/>
+    </row>
+    <row r="7" spans="1:18" s="239" customFormat="1" ht="40.049999999999997" customHeight="1">
+      <c r="A7" s="236"/>
+      <c r="B7" s="236"/>
+      <c r="C7" s="236"/>
+      <c r="D7" s="236"/>
+      <c r="E7" s="242"/>
+      <c r="F7" s="242"/>
+      <c r="G7" s="236"/>
+      <c r="H7" s="236"/>
+      <c r="I7" s="240"/>
+      <c r="J7" s="241"/>
+      <c r="K7" s="228"/>
+      <c r="L7" s="253"/>
+      <c r="M7" s="253"/>
+      <c r="N7" s="253"/>
+      <c r="O7" s="253"/>
+      <c r="P7" s="253"/>
+      <c r="Q7" s="253"/>
+      <c r="R7" s="254"/>
+    </row>
+    <row r="8" spans="1:18" s="239" customFormat="1" ht="40.049999999999997" customHeight="1">
+      <c r="A8" s="236"/>
+      <c r="B8" s="236"/>
+      <c r="C8" s="236"/>
+      <c r="D8" s="236"/>
+      <c r="E8" s="236"/>
+      <c r="F8" s="236"/>
+      <c r="G8" s="236"/>
+      <c r="H8" s="236"/>
+      <c r="I8" s="243"/>
+      <c r="J8" s="241"/>
+      <c r="K8" s="228"/>
+      <c r="L8" s="253"/>
+      <c r="M8" s="253"/>
+      <c r="N8" s="253"/>
+      <c r="O8" s="253"/>
+      <c r="P8" s="253"/>
+      <c r="Q8" s="253"/>
+      <c r="R8" s="254"/>
+    </row>
+    <row r="9" spans="1:18" s="239" customFormat="1" ht="40.049999999999997" customHeight="1">
+      <c r="A9" s="236"/>
+      <c r="B9" s="236"/>
+      <c r="C9" s="236"/>
+      <c r="D9" s="236"/>
+      <c r="E9" s="236"/>
+      <c r="F9" s="236"/>
+      <c r="G9" s="236"/>
+      <c r="H9" s="236"/>
+      <c r="I9" s="240"/>
+      <c r="J9" s="241"/>
+      <c r="K9" s="228"/>
+      <c r="L9" s="253"/>
+      <c r="M9" s="253"/>
+      <c r="N9" s="253"/>
+      <c r="O9" s="253"/>
+      <c r="P9" s="253"/>
+      <c r="Q9" s="253"/>
+      <c r="R9" s="254"/>
+    </row>
+    <row r="10" spans="1:18" s="239" customFormat="1" ht="40.049999999999997" customHeight="1">
+      <c r="A10" s="235"/>
+      <c r="B10" s="235"/>
+      <c r="C10" s="236"/>
+      <c r="D10" s="236"/>
+      <c r="E10" s="236"/>
+      <c r="F10" s="236"/>
+      <c r="G10" s="236"/>
+      <c r="H10" s="236"/>
+      <c r="I10" s="240"/>
+      <c r="J10" s="241"/>
+      <c r="K10" s="228"/>
+      <c r="L10" s="253"/>
+      <c r="M10" s="253"/>
+      <c r="N10" s="253"/>
+      <c r="O10" s="253"/>
+      <c r="P10" s="253"/>
+      <c r="Q10" s="253"/>
+      <c r="R10" s="254"/>
+    </row>
+    <row r="11" spans="1:18" s="239" customFormat="1" ht="40.049999999999997" customHeight="1">
+      <c r="A11" s="235"/>
+      <c r="B11" s="235"/>
+      <c r="C11" s="236"/>
+      <c r="D11" s="236"/>
+      <c r="E11" s="236"/>
+      <c r="F11" s="236"/>
+      <c r="G11" s="236"/>
+      <c r="H11" s="236"/>
+      <c r="I11" s="240"/>
+      <c r="J11" s="238"/>
+      <c r="K11" s="228"/>
+      <c r="L11" s="253"/>
+      <c r="M11" s="253"/>
+      <c r="N11" s="253"/>
+      <c r="O11" s="253"/>
+      <c r="P11" s="253"/>
+      <c r="Q11" s="253"/>
+      <c r="R11" s="254"/>
+    </row>
+    <row r="12" spans="1:18" s="239" customFormat="1" ht="40.049999999999997" customHeight="1">
+      <c r="A12" s="236"/>
+      <c r="B12" s="236"/>
+      <c r="C12" s="236"/>
+      <c r="D12" s="236"/>
+      <c r="E12" s="236"/>
+      <c r="F12" s="236"/>
+      <c r="G12" s="236"/>
+      <c r="H12" s="228"/>
+      <c r="I12" s="240"/>
+      <c r="J12" s="238"/>
+      <c r="K12" s="228"/>
+      <c r="L12" s="253"/>
+      <c r="M12" s="253"/>
+      <c r="N12" s="253"/>
+      <c r="O12" s="253"/>
+      <c r="P12" s="253"/>
+      <c r="Q12" s="253"/>
+      <c r="R12" s="254"/>
+    </row>
+    <row r="13" spans="1:18" s="239" customFormat="1" ht="40.049999999999997" customHeight="1">
+      <c r="A13" s="236"/>
+      <c r="B13" s="236"/>
+      <c r="C13" s="236"/>
+      <c r="D13" s="236"/>
+      <c r="E13" s="236"/>
+      <c r="F13" s="236"/>
+      <c r="G13" s="236"/>
+      <c r="H13" s="236"/>
+      <c r="I13" s="240"/>
+      <c r="J13" s="241"/>
+      <c r="K13" s="228"/>
+      <c r="L13" s="253"/>
+      <c r="M13" s="253"/>
+      <c r="N13" s="253"/>
+      <c r="O13" s="253"/>
+      <c r="P13" s="253"/>
+      <c r="Q13" s="253"/>
+      <c r="R13" s="254"/>
+    </row>
+    <row r="14" spans="1:18" s="239" customFormat="1" ht="40.049999999999997" customHeight="1">
+      <c r="A14" s="236"/>
+      <c r="B14" s="236"/>
+      <c r="C14" s="236"/>
+      <c r="D14" s="236"/>
+      <c r="E14" s="236"/>
+      <c r="F14" s="236"/>
+      <c r="G14" s="235"/>
+      <c r="H14" s="235"/>
+      <c r="I14" s="243"/>
+      <c r="J14" s="238"/>
+      <c r="K14" s="228"/>
+      <c r="L14" s="253"/>
+      <c r="M14" s="253"/>
+      <c r="N14" s="253"/>
+      <c r="O14" s="253"/>
+      <c r="P14" s="253"/>
+      <c r="Q14" s="253"/>
+      <c r="R14" s="254"/>
+    </row>
+    <row r="15" spans="1:18" s="239" customFormat="1" ht="40.049999999999997" customHeight="1">
+      <c r="A15" s="235"/>
+      <c r="B15" s="235"/>
+      <c r="C15" s="236"/>
+      <c r="D15" s="236"/>
+      <c r="E15" s="236"/>
+      <c r="F15" s="236"/>
+      <c r="G15" s="236"/>
+      <c r="H15" s="236"/>
+      <c r="I15" s="240"/>
+      <c r="J15" s="241"/>
+      <c r="K15" s="228"/>
+      <c r="L15" s="253"/>
+      <c r="M15" s="253"/>
+      <c r="N15" s="253"/>
+      <c r="O15" s="253"/>
+      <c r="P15" s="253"/>
+      <c r="Q15" s="253"/>
+      <c r="R15" s="254"/>
+    </row>
+    <row r="16" spans="1:18" s="239" customFormat="1" ht="40.049999999999997" customHeight="1">
+      <c r="A16" s="235"/>
+      <c r="B16" s="235"/>
+      <c r="C16" s="236"/>
+      <c r="D16" s="236"/>
+      <c r="E16" s="236"/>
+      <c r="F16" s="236"/>
+      <c r="G16" s="238"/>
+      <c r="H16" s="238"/>
+      <c r="I16" s="240"/>
+      <c r="J16" s="241"/>
+      <c r="K16" s="228"/>
+      <c r="L16" s="253"/>
+      <c r="M16" s="253"/>
+      <c r="N16" s="253"/>
+      <c r="O16" s="253"/>
+      <c r="P16" s="253"/>
+      <c r="Q16" s="253"/>
+      <c r="R16" s="254"/>
+    </row>
+    <row r="17" spans="1:18" s="239" customFormat="1" ht="40.049999999999997" customHeight="1">
+      <c r="A17" s="235"/>
+      <c r="B17" s="235"/>
+      <c r="C17" s="236"/>
+      <c r="D17" s="236"/>
+      <c r="E17" s="236"/>
+      <c r="F17" s="236"/>
+      <c r="G17" s="236"/>
+      <c r="H17" s="236"/>
+      <c r="I17" s="240"/>
+      <c r="J17" s="241"/>
+      <c r="K17" s="228"/>
+      <c r="L17" s="253"/>
+      <c r="M17" s="253"/>
+      <c r="N17" s="253"/>
+      <c r="O17" s="253"/>
+      <c r="P17" s="253"/>
+      <c r="Q17" s="253"/>
+      <c r="R17" s="254"/>
+    </row>
+    <row r="18" spans="1:18" s="239" customFormat="1" ht="40.049999999999997" customHeight="1">
+      <c r="A18" s="236"/>
+      <c r="B18" s="236"/>
+      <c r="C18" s="236"/>
+      <c r="D18" s="236"/>
+      <c r="E18" s="236"/>
+      <c r="F18" s="236"/>
+      <c r="G18" s="236"/>
+      <c r="H18" s="236"/>
+      <c r="I18" s="244"/>
+      <c r="J18" s="240"/>
+      <c r="K18" s="228"/>
+      <c r="L18" s="253"/>
+      <c r="M18" s="253"/>
+      <c r="N18" s="253"/>
+      <c r="O18" s="253"/>
+      <c r="P18" s="253"/>
+      <c r="Q18" s="253"/>
+      <c r="R18" s="254"/>
+    </row>
+    <row r="19" spans="1:18" s="239" customFormat="1" ht="40.049999999999997" customHeight="1">
+      <c r="A19" s="235"/>
+      <c r="B19" s="235"/>
+      <c r="C19" s="236"/>
+      <c r="D19" s="236"/>
+      <c r="E19" s="236"/>
+      <c r="F19" s="236"/>
+      <c r="G19" s="236"/>
+      <c r="H19" s="236"/>
+      <c r="I19" s="240"/>
+      <c r="J19" s="241"/>
+      <c r="K19" s="228"/>
+      <c r="L19" s="253"/>
+      <c r="M19" s="253"/>
+      <c r="N19" s="253"/>
+      <c r="O19" s="253"/>
+      <c r="P19" s="253"/>
+      <c r="Q19" s="253"/>
+      <c r="R19" s="254"/>
+    </row>
+    <row r="20" spans="1:18" s="239" customFormat="1" ht="40.049999999999997" customHeight="1">
+      <c r="A20" s="235"/>
+      <c r="B20" s="235"/>
+      <c r="C20" s="236"/>
+      <c r="D20" s="236"/>
+      <c r="E20" s="242"/>
+      <c r="F20" s="242"/>
+      <c r="G20" s="236"/>
+      <c r="H20" s="236"/>
+      <c r="I20" s="240"/>
+      <c r="J20" s="241"/>
+      <c r="K20" s="228"/>
+      <c r="L20" s="253"/>
+      <c r="M20" s="253"/>
+      <c r="N20" s="253"/>
+      <c r="O20" s="253"/>
+      <c r="P20" s="253"/>
+      <c r="Q20" s="253"/>
+      <c r="R20" s="254"/>
+    </row>
+    <row r="21" spans="1:18" s="239" customFormat="1" ht="40.049999999999997" customHeight="1">
+      <c r="A21" s="235"/>
+      <c r="B21" s="235"/>
+      <c r="C21" s="236"/>
+      <c r="D21" s="236"/>
+      <c r="E21" s="236"/>
+      <c r="F21" s="236"/>
+      <c r="G21" s="236"/>
+      <c r="H21" s="236"/>
+      <c r="I21" s="240"/>
+      <c r="J21" s="241"/>
+      <c r="K21" s="228"/>
+      <c r="L21" s="253"/>
+      <c r="M21" s="253"/>
+      <c r="N21" s="253"/>
+      <c r="O21" s="253"/>
+      <c r="P21" s="253"/>
+      <c r="Q21" s="253"/>
+      <c r="R21" s="254"/>
+    </row>
+    <row r="22" spans="1:18" s="239" customFormat="1" ht="40.049999999999997" customHeight="1">
+      <c r="A22" s="235"/>
+      <c r="B22" s="235"/>
+      <c r="C22" s="236"/>
+      <c r="D22" s="236"/>
+      <c r="E22" s="236"/>
+      <c r="F22" s="236"/>
+      <c r="G22" s="236"/>
+      <c r="H22" s="236"/>
+      <c r="I22" s="240"/>
+      <c r="J22" s="241"/>
+      <c r="K22" s="228"/>
+      <c r="L22" s="253"/>
+      <c r="M22" s="253"/>
+      <c r="N22" s="253"/>
+      <c r="O22" s="253"/>
+      <c r="P22" s="253"/>
+      <c r="Q22" s="253"/>
+      <c r="R22" s="254"/>
+    </row>
+    <row r="23" spans="1:18" s="239" customFormat="1" ht="40.049999999999997" customHeight="1">
+      <c r="A23" s="235"/>
+      <c r="B23" s="235"/>
+      <c r="C23" s="236"/>
+      <c r="D23" s="236"/>
+      <c r="E23" s="236"/>
+      <c r="F23" s="236"/>
+      <c r="G23" s="236"/>
+      <c r="H23" s="236"/>
+      <c r="I23" s="240"/>
+      <c r="J23" s="241"/>
+      <c r="K23" s="228"/>
+      <c r="L23" s="253"/>
+      <c r="M23" s="253"/>
+      <c r="N23" s="253"/>
+      <c r="O23" s="253"/>
+      <c r="P23" s="253"/>
+      <c r="Q23" s="253"/>
+      <c r="R23" s="254"/>
+    </row>
+    <row r="24" spans="1:18" s="239" customFormat="1" ht="40.049999999999997" customHeight="1">
+      <c r="A24" s="235"/>
+      <c r="B24" s="235"/>
+      <c r="C24" s="236"/>
+      <c r="D24" s="236"/>
+      <c r="E24" s="236"/>
+      <c r="F24" s="236"/>
+      <c r="G24" s="236"/>
+      <c r="H24" s="236"/>
+      <c r="I24" s="240"/>
+      <c r="J24" s="241"/>
+      <c r="K24" s="228"/>
+      <c r="L24" s="253"/>
+      <c r="M24" s="253"/>
+      <c r="N24" s="253"/>
+      <c r="O24" s="253"/>
+      <c r="P24" s="253"/>
+      <c r="Q24" s="253"/>
+      <c r="R24" s="254"/>
+    </row>
+    <row r="25" spans="1:18" s="239" customFormat="1" ht="40.049999999999997" customHeight="1">
+      <c r="A25" s="235"/>
+      <c r="B25" s="235"/>
+      <c r="C25" s="236"/>
+      <c r="D25" s="236"/>
+      <c r="E25" s="236"/>
+      <c r="F25" s="236"/>
+      <c r="G25" s="236"/>
+      <c r="H25" s="236"/>
+      <c r="I25" s="240"/>
+      <c r="J25" s="241"/>
+      <c r="K25" s="228"/>
+      <c r="L25" s="253"/>
+      <c r="M25" s="253"/>
+      <c r="N25" s="253"/>
+      <c r="O25" s="253"/>
+      <c r="P25" s="253"/>
+      <c r="Q25" s="253"/>
+      <c r="R25" s="254"/>
+    </row>
+    <row r="26" spans="1:18" s="239" customFormat="1" ht="40.049999999999997" customHeight="1">
+      <c r="A26" s="236"/>
+      <c r="B26" s="236"/>
+      <c r="C26" s="236"/>
+      <c r="D26" s="236"/>
+      <c r="E26" s="236"/>
+      <c r="F26" s="236"/>
+      <c r="G26" s="236"/>
+      <c r="H26" s="236"/>
+      <c r="I26" s="240"/>
+      <c r="J26" s="241"/>
+      <c r="K26" s="228"/>
+      <c r="L26" s="253"/>
+      <c r="M26" s="253"/>
+      <c r="N26" s="253"/>
+      <c r="O26" s="253"/>
+      <c r="P26" s="253"/>
+      <c r="Q26" s="253"/>
+      <c r="R26" s="254"/>
+    </row>
+    <row r="27" spans="1:18" ht="25.2">
+      <c r="C27" s="225"/>
+      <c r="D27" s="224"/>
+      <c r="E27" s="223"/>
+      <c r="F27" s="223"/>
+      <c r="G27" s="220"/>
+      <c r="L27" s="255"/>
+      <c r="M27" s="255"/>
+      <c r="N27" s="255"/>
+      <c r="O27" s="255"/>
+      <c r="P27" s="255"/>
+      <c r="Q27" s="255"/>
+      <c r="R27" s="256"/>
+    </row>
+    <row r="28" spans="1:18" ht="23.4">
+      <c r="L28" s="255"/>
+      <c r="M28" s="255"/>
+      <c r="N28" s="255"/>
+      <c r="O28" s="255"/>
+      <c r="P28" s="255"/>
+      <c r="Q28" s="255"/>
+      <c r="R28" s="256"/>
+    </row>
+    <row r="29" spans="1:18" ht="23.4">
+      <c r="L29" s="255"/>
+      <c r="M29" s="255"/>
+      <c r="N29" s="255"/>
+      <c r="O29" s="255"/>
+      <c r="P29" s="255"/>
+      <c r="Q29" s="255"/>
+      <c r="R29" s="256"/>
+    </row>
+    <row r="30" spans="1:18" ht="23.4">
+      <c r="L30" s="255"/>
+      <c r="M30" s="255"/>
+      <c r="N30" s="255"/>
+      <c r="O30" s="255"/>
+      <c r="P30" s="255"/>
+      <c r="Q30" s="255"/>
+      <c r="R30" s="256"/>
+    </row>
+    <row r="31" spans="1:18" ht="23.4">
+      <c r="L31" s="255"/>
+      <c r="M31" s="255"/>
+      <c r="N31" s="255"/>
+      <c r="O31" s="255"/>
+      <c r="P31" s="255"/>
+      <c r="Q31" s="255"/>
+      <c r="R31" s="256"/>
+    </row>
+    <row r="32" spans="1:18" ht="23.4">
+      <c r="L32" s="255"/>
+      <c r="M32" s="255"/>
+      <c r="N32" s="255"/>
+      <c r="O32" s="255"/>
+      <c r="P32" s="255"/>
+      <c r="Q32" s="255"/>
+      <c r="R32" s="256"/>
+    </row>
+    <row r="33" spans="12:18" ht="23.4">
+      <c r="L33" s="255"/>
+      <c r="M33" s="255"/>
+      <c r="N33" s="255"/>
+      <c r="O33" s="255"/>
+      <c r="P33" s="255"/>
+      <c r="Q33" s="255"/>
+      <c r="R33" s="256"/>
+    </row>
+    <row r="34" spans="12:18" ht="23.4">
+      <c r="L34" s="255"/>
+      <c r="M34" s="255"/>
+      <c r="N34" s="255"/>
+      <c r="O34" s="255"/>
+      <c r="P34" s="255"/>
+      <c r="Q34" s="255"/>
+      <c r="R34" s="256"/>
+    </row>
+    <row r="35" spans="12:18" ht="23.4">
+      <c r="L35" s="255"/>
+      <c r="M35" s="255"/>
+      <c r="N35" s="255"/>
+      <c r="O35" s="255"/>
+      <c r="P35" s="255"/>
+      <c r="Q35" s="255"/>
+      <c r="R35" s="256"/>
+    </row>
+    <row r="36" spans="12:18" ht="23.4">
+      <c r="L36" s="255"/>
+      <c r="M36" s="255"/>
+      <c r="N36" s="255"/>
+      <c r="O36" s="255"/>
+      <c r="P36" s="255"/>
+      <c r="Q36" s="255"/>
+      <c r="R36" s="256"/>
+    </row>
+    <row r="37" spans="12:18" ht="23.4">
+      <c r="L37" s="255"/>
+      <c r="M37" s="255"/>
+      <c r="N37" s="255"/>
+      <c r="O37" s="255"/>
+      <c r="P37" s="255"/>
+      <c r="Q37" s="255"/>
+      <c r="R37" s="256"/>
+    </row>
+    <row r="38" spans="12:18" ht="23.4">
+      <c r="L38" s="255"/>
+      <c r="M38" s="255"/>
+      <c r="N38" s="255"/>
+      <c r="O38" s="255"/>
+      <c r="P38" s="255"/>
+      <c r="Q38" s="255"/>
+      <c r="R38" s="256"/>
+    </row>
+    <row r="39" spans="12:18" ht="23.4">
+      <c r="L39" s="255"/>
+      <c r="M39" s="255"/>
+      <c r="N39" s="255"/>
+      <c r="O39" s="255"/>
+      <c r="P39" s="255"/>
+      <c r="Q39" s="255"/>
+      <c r="R39" s="256"/>
+    </row>
+    <row r="40" spans="12:18" ht="23.4">
+      <c r="L40" s="255"/>
+      <c r="M40" s="255"/>
+      <c r="N40" s="255"/>
+      <c r="O40" s="255"/>
+      <c r="P40" s="255"/>
+      <c r="Q40" s="255"/>
+      <c r="R40" s="256"/>
+    </row>
+    <row r="41" spans="12:18" ht="23.4">
+      <c r="L41" s="255"/>
+      <c r="M41" s="255"/>
+      <c r="N41" s="255"/>
+      <c r="O41" s="255"/>
+      <c r="P41" s="255"/>
+      <c r="Q41" s="255"/>
+      <c r="R41" s="256"/>
+    </row>
+    <row r="42" spans="12:18" ht="23.4">
+      <c r="L42" s="255"/>
+      <c r="M42" s="255"/>
+      <c r="N42" s="255"/>
+      <c r="O42" s="255"/>
+      <c r="P42" s="255"/>
+      <c r="Q42" s="255"/>
+      <c r="R42" s="256"/>
+    </row>
+    <row r="43" spans="12:18" ht="23.4">
+      <c r="L43" s="255"/>
+      <c r="M43" s="255"/>
+      <c r="N43" s="255"/>
+      <c r="O43" s="255"/>
+      <c r="P43" s="255"/>
+      <c r="Q43" s="255"/>
+      <c r="R43" s="256"/>
+    </row>
+    <row r="44" spans="12:18" ht="23.4">
+      <c r="L44" s="255"/>
+      <c r="M44" s="255"/>
+      <c r="N44" s="255"/>
+      <c r="O44" s="255"/>
+      <c r="P44" s="255"/>
+      <c r="Q44" s="255"/>
+      <c r="R44" s="256"/>
+    </row>
+    <row r="45" spans="12:18" ht="23.4">
+      <c r="L45" s="255"/>
+      <c r="M45" s="255"/>
+      <c r="N45" s="255"/>
+      <c r="O45" s="255"/>
+      <c r="P45" s="255"/>
+      <c r="Q45" s="255"/>
+      <c r="R45" s="256"/>
+    </row>
+    <row r="46" spans="12:18" ht="23.4">
+      <c r="L46" s="255"/>
+      <c r="M46" s="255"/>
+      <c r="N46" s="255"/>
+      <c r="O46" s="255"/>
+      <c r="P46" s="255"/>
+      <c r="Q46" s="255"/>
+      <c r="R46" s="256"/>
+    </row>
+    <row r="47" spans="12:18" ht="23.4">
+      <c r="L47" s="255"/>
+      <c r="M47" s="255"/>
+      <c r="N47" s="255"/>
+      <c r="O47" s="255"/>
+      <c r="P47" s="255"/>
+      <c r="Q47" s="255"/>
+      <c r="R47" s="256"/>
+    </row>
+    <row r="48" spans="12:18" ht="23.4">
+      <c r="L48" s="255"/>
+      <c r="M48" s="255"/>
+      <c r="N48" s="255"/>
+      <c r="O48" s="255"/>
+      <c r="P48" s="255"/>
+      <c r="Q48" s="255"/>
+      <c r="R48" s="256"/>
+    </row>
+    <row r="49" spans="12:18" ht="23.4">
+      <c r="L49" s="255"/>
+      <c r="M49" s="255"/>
+      <c r="N49" s="255"/>
+      <c r="O49" s="255"/>
+      <c r="P49" s="255"/>
+      <c r="Q49" s="255"/>
+      <c r="R49" s="256"/>
+    </row>
+    <row r="50" spans="12:18" ht="23.4">
+      <c r="L50" s="255"/>
+      <c r="M50" s="255"/>
+      <c r="N50" s="255"/>
+      <c r="O50" s="255"/>
+      <c r="P50" s="255"/>
+      <c r="Q50" s="255"/>
+      <c r="R50" s="256"/>
+    </row>
+    <row r="51" spans="12:18" ht="23.4">
+      <c r="L51" s="255"/>
+      <c r="M51" s="255"/>
+      <c r="N51" s="255"/>
+      <c r="O51" s="255"/>
+      <c r="P51" s="255"/>
+      <c r="Q51" s="255"/>
+      <c r="R51" s="256"/>
+    </row>
+    <row r="52" spans="12:18" ht="23.4">
+      <c r="L52" s="255"/>
+      <c r="M52" s="255"/>
+      <c r="N52" s="255"/>
+      <c r="O52" s="255"/>
+      <c r="P52" s="255"/>
+      <c r="Q52" s="255"/>
+      <c r="R52" s="256"/>
+    </row>
+    <row r="53" spans="12:18" ht="23.4">
+      <c r="L53" s="255"/>
+      <c r="M53" s="255"/>
+      <c r="N53" s="255"/>
+      <c r="O53" s="255"/>
+      <c r="P53" s="255"/>
+      <c r="Q53" s="255"/>
+      <c r="R53" s="256"/>
+    </row>
+    <row r="54" spans="12:18" ht="23.4">
+      <c r="L54" s="255"/>
+      <c r="M54" s="255"/>
+      <c r="N54" s="255"/>
+      <c r="O54" s="255"/>
+      <c r="P54" s="255"/>
+      <c r="Q54" s="255"/>
+      <c r="R54" s="256"/>
+    </row>
+    <row r="55" spans="12:18" ht="23.4">
+      <c r="L55" s="255"/>
+      <c r="M55" s="255"/>
+      <c r="N55" s="255"/>
+      <c r="O55" s="255"/>
+      <c r="P55" s="255"/>
+      <c r="Q55" s="255"/>
+      <c r="R55" s="256"/>
+    </row>
+    <row r="56" spans="12:18" ht="23.4">
+      <c r="L56" s="255"/>
+      <c r="M56" s="255"/>
+      <c r="N56" s="255"/>
+      <c r="O56" s="255"/>
+      <c r="P56" s="255"/>
+      <c r="Q56" s="255"/>
+      <c r="R56" s="256"/>
+    </row>
+    <row r="57" spans="12:18" ht="23.4">
+      <c r="L57" s="255"/>
+      <c r="M57" s="255"/>
+      <c r="N57" s="255"/>
+      <c r="O57" s="255"/>
+      <c r="P57" s="255"/>
+      <c r="Q57" s="255"/>
+      <c r="R57" s="256"/>
+    </row>
+    <row r="58" spans="12:18" ht="23.4">
+      <c r="L58" s="255"/>
+      <c r="M58" s="255"/>
+      <c r="N58" s="255"/>
+      <c r="O58" s="255"/>
+      <c r="P58" s="255"/>
+      <c r="Q58" s="255"/>
+      <c r="R58" s="256"/>
+    </row>
+    <row r="59" spans="12:18" ht="23.4">
+      <c r="L59" s="255"/>
+      <c r="M59" s="255"/>
+      <c r="N59" s="255"/>
+      <c r="O59" s="255"/>
+      <c r="P59" s="255"/>
+      <c r="Q59" s="255"/>
+      <c r="R59" s="256"/>
+    </row>
+    <row r="60" spans="12:18" ht="23.4">
+      <c r="L60" s="255"/>
+      <c r="M60" s="255"/>
+      <c r="N60" s="255"/>
+      <c r="O60" s="255"/>
+      <c r="P60" s="255"/>
+      <c r="Q60" s="255"/>
+      <c r="R60" s="256"/>
+    </row>
+    <row r="61" spans="12:18" ht="23.4">
+      <c r="L61" s="255"/>
+      <c r="M61" s="255"/>
+      <c r="N61" s="255"/>
+      <c r="O61" s="255"/>
+      <c r="P61" s="255"/>
+      <c r="Q61" s="255"/>
+      <c r="R61" s="256"/>
+    </row>
+    <row r="62" spans="12:18" ht="23.4">
+      <c r="L62" s="255"/>
+      <c r="M62" s="255"/>
+      <c r="N62" s="255"/>
+      <c r="O62" s="255"/>
+      <c r="P62" s="255"/>
+      <c r="Q62" s="255"/>
+      <c r="R62" s="256"/>
+    </row>
+    <row r="63" spans="12:18" ht="23.4">
+      <c r="L63" s="255"/>
+      <c r="M63" s="255"/>
+      <c r="N63" s="255"/>
+      <c r="O63" s="255"/>
+      <c r="P63" s="255"/>
+      <c r="Q63" s="255"/>
+      <c r="R63" s="256"/>
+    </row>
+    <row r="64" spans="12:18" ht="23.4">
+      <c r="L64" s="255"/>
+      <c r="M64" s="255"/>
+      <c r="N64" s="255"/>
+      <c r="O64" s="255"/>
+      <c r="P64" s="255"/>
+      <c r="Q64" s="255"/>
+      <c r="R64" s="256"/>
+    </row>
+    <row r="65" spans="12:18" ht="23.4">
+      <c r="L65" s="255"/>
+      <c r="M65" s="255"/>
+      <c r="N65" s="255"/>
+      <c r="O65" s="255"/>
+      <c r="P65" s="255"/>
+      <c r="Q65" s="255"/>
+      <c r="R65" s="256"/>
+    </row>
+    <row r="66" spans="12:18" ht="23.4">
+      <c r="L66" s="255"/>
+      <c r="M66" s="255"/>
+      <c r="N66" s="255"/>
+      <c r="O66" s="255"/>
+      <c r="P66" s="255"/>
+      <c r="Q66" s="255"/>
+      <c r="R66" s="256"/>
+    </row>
+    <row r="67" spans="12:18" ht="23.4">
+      <c r="L67" s="255"/>
+      <c r="M67" s="255"/>
+      <c r="N67" s="255"/>
+      <c r="O67" s="255"/>
+      <c r="P67" s="255"/>
+      <c r="Q67" s="255"/>
+      <c r="R67" s="256"/>
+    </row>
+    <row r="68" spans="12:18" ht="23.4">
+      <c r="L68" s="255"/>
+      <c r="M68" s="255"/>
+      <c r="N68" s="255"/>
+      <c r="O68" s="255"/>
+      <c r="P68" s="255"/>
+      <c r="Q68" s="255"/>
+      <c r="R68" s="256"/>
+    </row>
+    <row r="69" spans="12:18" ht="23.4">
+      <c r="L69" s="255"/>
+      <c r="M69" s="255"/>
+      <c r="N69" s="255"/>
+      <c r="O69" s="255"/>
+      <c r="P69" s="255"/>
+      <c r="Q69" s="255"/>
+      <c r="R69" s="256"/>
+    </row>
+    <row r="70" spans="12:18" ht="23.4">
+      <c r="L70" s="255"/>
+      <c r="M70" s="255"/>
+      <c r="N70" s="255"/>
+      <c r="O70" s="255"/>
+      <c r="P70" s="255"/>
+      <c r="Q70" s="255"/>
+      <c r="R70" s="256"/>
+    </row>
+    <row r="71" spans="12:18" ht="23.4">
+      <c r="L71" s="255"/>
+      <c r="M71" s="255"/>
+      <c r="N71" s="255"/>
+      <c r="O71" s="255"/>
+      <c r="P71" s="255"/>
+      <c r="Q71" s="255"/>
+      <c r="R71" s="256"/>
+    </row>
+    <row r="72" spans="12:18" ht="23.4">
+      <c r="L72" s="255"/>
+      <c r="M72" s="255"/>
+      <c r="N72" s="255"/>
+      <c r="O72" s="255"/>
+      <c r="P72" s="255"/>
+      <c r="Q72" s="255"/>
+      <c r="R72" s="256"/>
+    </row>
+    <row r="73" spans="12:18" ht="23.4">
+      <c r="L73" s="255"/>
+      <c r="M73" s="255"/>
+      <c r="N73" s="255"/>
+      <c r="O73" s="255"/>
+      <c r="P73" s="255"/>
+      <c r="Q73" s="255"/>
+      <c r="R73" s="256"/>
+    </row>
+    <row r="74" spans="12:18" ht="23.4">
+      <c r="L74" s="255"/>
+      <c r="M74" s="255"/>
+      <c r="N74" s="255"/>
+      <c r="O74" s="255"/>
+      <c r="P74" s="255"/>
+      <c r="Q74" s="255"/>
+      <c r="R74" s="256"/>
+    </row>
+    <row r="75" spans="12:18" ht="23.4">
+      <c r="L75" s="255"/>
+      <c r="M75" s="255"/>
+      <c r="N75" s="255"/>
+      <c r="O75" s="255"/>
+      <c r="P75" s="255"/>
+      <c r="Q75" s="255"/>
+      <c r="R75" s="256"/>
+    </row>
+    <row r="76" spans="12:18" ht="23.4">
+      <c r="L76" s="255"/>
+      <c r="M76" s="255"/>
+      <c r="N76" s="255"/>
+      <c r="O76" s="255"/>
+      <c r="P76" s="255"/>
+      <c r="Q76" s="255"/>
+      <c r="R76" s="256"/>
+    </row>
+    <row r="77" spans="12:18" ht="23.4">
+      <c r="L77" s="255"/>
+      <c r="M77" s="255"/>
+      <c r="N77" s="255"/>
+      <c r="O77" s="255"/>
+      <c r="P77" s="255"/>
+      <c r="Q77" s="255"/>
+      <c r="R77" s="256"/>
+    </row>
+    <row r="78" spans="12:18" ht="23.4">
+      <c r="L78" s="255"/>
+      <c r="M78" s="255"/>
+      <c r="N78" s="255"/>
+      <c r="O78" s="255"/>
+      <c r="P78" s="255"/>
+      <c r="Q78" s="255"/>
+      <c r="R78" s="256"/>
+    </row>
+    <row r="79" spans="12:18" ht="23.4">
+      <c r="L79" s="255"/>
+      <c r="M79" s="255"/>
+      <c r="N79" s="255"/>
+      <c r="O79" s="255"/>
+      <c r="P79" s="255"/>
+      <c r="Q79" s="255"/>
+      <c r="R79" s="256"/>
+    </row>
+    <row r="80" spans="12:18" ht="23.4">
+      <c r="L80" s="255"/>
+      <c r="M80" s="255"/>
+      <c r="N80" s="255"/>
+      <c r="O80" s="255"/>
+      <c r="P80" s="255"/>
+      <c r="Q80" s="255"/>
+      <c r="R80" s="256"/>
+    </row>
+    <row r="81" spans="12:18" ht="23.4">
+      <c r="L81" s="255"/>
+      <c r="M81" s="255"/>
+      <c r="N81" s="255"/>
+      <c r="O81" s="255"/>
+      <c r="P81" s="255"/>
+      <c r="Q81" s="255"/>
+      <c r="R81" s="256"/>
+    </row>
+    <row r="82" spans="12:18" ht="23.4">
+      <c r="L82" s="255"/>
+      <c r="M82" s="255"/>
+      <c r="N82" s="255"/>
+      <c r="O82" s="255"/>
+      <c r="P82" s="255"/>
+      <c r="Q82" s="255"/>
+      <c r="R82" s="256"/>
+    </row>
+    <row r="83" spans="12:18" ht="23.4">
+      <c r="L83" s="255"/>
+      <c r="M83" s="255"/>
+      <c r="N83" s="255"/>
+      <c r="O83" s="255"/>
+      <c r="P83" s="255"/>
+      <c r="Q83" s="255"/>
+      <c r="R83" s="256"/>
+    </row>
+    <row r="84" spans="12:18" ht="23.4">
+      <c r="L84" s="255"/>
+      <c r="M84" s="255"/>
+      <c r="N84" s="255"/>
+      <c r="O84" s="255"/>
+      <c r="P84" s="255"/>
+      <c r="Q84" s="255"/>
+      <c r="R84" s="256"/>
+    </row>
+    <row r="85" spans="12:18" ht="23.4">
+      <c r="L85" s="255"/>
+      <c r="M85" s="255"/>
+      <c r="N85" s="255"/>
+      <c r="O85" s="255"/>
+      <c r="P85" s="255"/>
+      <c r="Q85" s="255"/>
+      <c r="R85" s="256"/>
+    </row>
+    <row r="86" spans="12:18" ht="23.4">
+      <c r="L86" s="255"/>
+      <c r="M86" s="255"/>
+      <c r="N86" s="255"/>
+      <c r="O86" s="255"/>
+      <c r="P86" s="255"/>
+      <c r="Q86" s="255"/>
+      <c r="R86" s="256"/>
+    </row>
+    <row r="87" spans="12:18" ht="23.4">
+      <c r="L87" s="255"/>
+      <c r="M87" s="255"/>
+      <c r="N87" s="255"/>
+      <c r="O87" s="255"/>
+      <c r="P87" s="255"/>
+      <c r="Q87" s="255"/>
+      <c r="R87" s="256"/>
+    </row>
+    <row r="88" spans="12:18" ht="23.4">
+      <c r="L88" s="255"/>
+      <c r="M88" s="255"/>
+      <c r="N88" s="255"/>
+      <c r="O88" s="255"/>
+      <c r="P88" s="255"/>
+      <c r="Q88" s="255"/>
+      <c r="R88" s="256"/>
+    </row>
+    <row r="89" spans="12:18" ht="23.4">
+      <c r="L89" s="255"/>
+      <c r="M89" s="255"/>
+      <c r="N89" s="255"/>
+      <c r="O89" s="255"/>
+      <c r="P89" s="255"/>
+      <c r="Q89" s="255"/>
+      <c r="R89" s="256"/>
+    </row>
+    <row r="90" spans="12:18" ht="23.4">
+      <c r="L90" s="255"/>
+      <c r="M90" s="255"/>
+      <c r="N90" s="255"/>
+      <c r="O90" s="255"/>
+      <c r="P90" s="255"/>
+      <c r="Q90" s="255"/>
+      <c r="R90" s="256"/>
+    </row>
+    <row r="91" spans="12:18" ht="23.4">
+      <c r="L91" s="255"/>
+      <c r="M91" s="255"/>
+      <c r="N91" s="255"/>
+      <c r="O91" s="255"/>
+      <c r="P91" s="255"/>
+      <c r="Q91" s="255"/>
+      <c r="R91" s="256"/>
+    </row>
+    <row r="92" spans="12:18" ht="23.4">
+      <c r="L92" s="255"/>
+      <c r="M92" s="255"/>
+      <c r="N92" s="255"/>
+      <c r="O92" s="255"/>
+      <c r="P92" s="255"/>
+      <c r="Q92" s="255"/>
+      <c r="R92" s="256"/>
+    </row>
+    <row r="93" spans="12:18" ht="23.4">
+      <c r="L93" s="255"/>
+      <c r="M93" s="255"/>
+      <c r="N93" s="255"/>
+      <c r="O93" s="255"/>
+      <c r="P93" s="255"/>
+      <c r="Q93" s="255"/>
+      <c r="R93" s="256"/>
+    </row>
+    <row r="94" spans="12:18" ht="23.4">
+      <c r="L94" s="255"/>
+      <c r="M94" s="255"/>
+      <c r="N94" s="255"/>
+      <c r="O94" s="255"/>
+      <c r="P94" s="255"/>
+      <c r="Q94" s="255"/>
+      <c r="R94" s="256"/>
+    </row>
+    <row r="95" spans="12:18" ht="23.4">
+      <c r="L95" s="255"/>
+      <c r="M95" s="255"/>
+      <c r="N95" s="255"/>
+      <c r="O95" s="255"/>
+      <c r="P95" s="255"/>
+      <c r="Q95" s="255"/>
+      <c r="R95" s="256"/>
+    </row>
+    <row r="96" spans="12:18" ht="23.4">
+      <c r="L96" s="255"/>
+      <c r="M96" s="255"/>
+      <c r="N96" s="255"/>
+      <c r="O96" s="255"/>
+      <c r="P96" s="255"/>
+      <c r="Q96" s="255"/>
+      <c r="R96" s="256"/>
+    </row>
+    <row r="97" spans="12:18" ht="23.4">
+      <c r="L97" s="255"/>
+      <c r="M97" s="255"/>
+      <c r="N97" s="255"/>
+      <c r="O97" s="255"/>
+      <c r="P97" s="255"/>
+      <c r="Q97" s="255"/>
+      <c r="R97" s="256"/>
+    </row>
+    <row r="98" spans="12:18" ht="23.4">
+      <c r="L98" s="255"/>
+      <c r="M98" s="255"/>
+      <c r="N98" s="255"/>
+      <c r="O98" s="255"/>
+      <c r="P98" s="255"/>
+      <c r="Q98" s="255"/>
+      <c r="R98" s="256"/>
+    </row>
+    <row r="99" spans="12:18" ht="23.4">
+      <c r="L99" s="255"/>
+      <c r="M99" s="255"/>
+      <c r="N99" s="255"/>
+      <c r="O99" s="255"/>
+      <c r="P99" s="255"/>
+      <c r="Q99" s="255"/>
+      <c r="R99" s="256"/>
+    </row>
+    <row r="100" spans="12:18" ht="23.4">
+      <c r="L100" s="255"/>
+      <c r="M100" s="255"/>
+      <c r="N100" s="255"/>
+      <c r="O100" s="255"/>
+      <c r="P100" s="255"/>
+      <c r="Q100" s="255"/>
+      <c r="R100" s="256"/>
+    </row>
+    <row r="101" spans="12:18" ht="23.4">
+      <c r="L101" s="255"/>
+      <c r="M101" s="255"/>
+      <c r="N101" s="255"/>
+      <c r="O101" s="255"/>
+      <c r="P101" s="255"/>
+      <c r="Q101" s="255"/>
+      <c r="R101" s="256"/>
+    </row>
+    <row r="102" spans="12:18" ht="23.4">
+      <c r="L102" s="255"/>
+      <c r="M102" s="255"/>
+      <c r="N102" s="255"/>
+      <c r="O102" s="255"/>
+      <c r="P102" s="255"/>
+      <c r="Q102" s="255"/>
+      <c r="R102" s="256"/>
+    </row>
+    <row r="103" spans="12:18" ht="23.4">
+      <c r="L103" s="255"/>
+      <c r="M103" s="255"/>
+      <c r="N103" s="255"/>
+      <c r="O103" s="255"/>
+      <c r="P103" s="255"/>
+      <c r="Q103" s="255"/>
+      <c r="R103" s="256"/>
+    </row>
+    <row r="104" spans="12:18" ht="23.4">
+      <c r="L104" s="255"/>
+      <c r="M104" s="255"/>
+      <c r="N104" s="255"/>
+      <c r="O104" s="255"/>
+      <c r="P104" s="255"/>
+      <c r="Q104" s="255"/>
+      <c r="R104" s="256"/>
+    </row>
+    <row r="105" spans="12:18" ht="23.4">
+      <c r="L105" s="255"/>
+      <c r="M105" s="255"/>
+      <c r="N105" s="255"/>
+      <c r="O105" s="255"/>
+      <c r="P105" s="255"/>
+      <c r="Q105" s="255"/>
+      <c r="R105" s="256"/>
+    </row>
+    <row r="106" spans="12:18" ht="23.4">
+      <c r="L106" s="255"/>
+      <c r="M106" s="255"/>
+      <c r="N106" s="255"/>
+      <c r="O106" s="255"/>
+      <c r="P106" s="255"/>
+      <c r="Q106" s="255"/>
+      <c r="R106" s="256"/>
+    </row>
+    <row r="107" spans="12:18" ht="23.4">
+      <c r="L107" s="255"/>
+      <c r="M107" s="255"/>
+      <c r="N107" s="255"/>
+      <c r="O107" s="255"/>
+      <c r="P107" s="255"/>
+      <c r="Q107" s="255"/>
+      <c r="R107" s="256"/>
+    </row>
+    <row r="108" spans="12:18" ht="23.4">
+      <c r="L108" s="255"/>
+      <c r="M108" s="255"/>
+      <c r="N108" s="255"/>
+      <c r="O108" s="255"/>
+      <c r="P108" s="255"/>
+      <c r="Q108" s="255"/>
+      <c r="R108" s="256"/>
+    </row>
+    <row r="109" spans="12:18" ht="23.4">
+      <c r="L109" s="255"/>
+      <c r="M109" s="255"/>
+      <c r="N109" s="255"/>
+      <c r="O109" s="255"/>
+      <c r="P109" s="255"/>
+      <c r="Q109" s="255"/>
+      <c r="R109" s="256"/>
+    </row>
+    <row r="110" spans="12:18" ht="23.4">
+      <c r="L110" s="255"/>
+      <c r="M110" s="255"/>
+      <c r="N110" s="255"/>
+      <c r="O110" s="255"/>
+      <c r="P110" s="255"/>
+      <c r="Q110" s="255"/>
+      <c r="R110" s="256"/>
+    </row>
+    <row r="111" spans="12:18" ht="23.4">
+      <c r="L111" s="255"/>
+      <c r="M111" s="255"/>
+      <c r="N111" s="255"/>
+      <c r="O111" s="255"/>
+      <c r="P111" s="255"/>
+      <c r="Q111" s="255"/>
+      <c r="R111" s="256"/>
+    </row>
+    <row r="112" spans="12:18" ht="23.4">
+      <c r="L112" s="255"/>
+      <c r="M112" s="255"/>
+      <c r="N112" s="255"/>
+      <c r="O112" s="255"/>
+      <c r="P112" s="255"/>
+      <c r="Q112" s="255"/>
+      <c r="R112" s="256"/>
+    </row>
+    <row r="113" spans="12:18" ht="23.4">
+      <c r="L113" s="255"/>
+      <c r="M113" s="255"/>
+      <c r="N113" s="255"/>
+      <c r="O113" s="255"/>
+      <c r="P113" s="255"/>
+      <c r="Q113" s="255"/>
+      <c r="R113" s="256"/>
+    </row>
+    <row r="114" spans="12:18" ht="23.4">
+      <c r="L114" s="255"/>
+      <c r="M114" s="255"/>
+      <c r="N114" s="255"/>
+      <c r="O114" s="255"/>
+      <c r="P114" s="255"/>
+      <c r="Q114" s="255"/>
+      <c r="R114" s="256"/>
+    </row>
+    <row r="115" spans="12:18" ht="23.4">
+      <c r="L115" s="255"/>
+      <c r="M115" s="255"/>
+      <c r="N115" s="255"/>
+      <c r="O115" s="255"/>
+      <c r="P115" s="255"/>
+      <c r="Q115" s="255"/>
+      <c r="R115" s="256"/>
+    </row>
+    <row r="116" spans="12:18" ht="23.4">
+      <c r="L116" s="255"/>
+      <c r="M116" s="255"/>
+      <c r="N116" s="255"/>
+      <c r="O116" s="255"/>
+      <c r="P116" s="255"/>
+      <c r="Q116" s="255"/>
+      <c r="R116" s="256"/>
+    </row>
+    <row r="117" spans="12:18" ht="23.4">
+      <c r="L117" s="255"/>
+      <c r="M117" s="255"/>
+      <c r="N117" s="255"/>
+      <c r="O117" s="255"/>
+      <c r="P117" s="255"/>
+      <c r="Q117" s="255"/>
+      <c r="R117" s="256"/>
+    </row>
+    <row r="118" spans="12:18" ht="23.4">
+      <c r="L118" s="255"/>
+      <c r="M118" s="255"/>
+      <c r="N118" s="255"/>
+      <c r="O118" s="255"/>
+      <c r="P118" s="255"/>
+      <c r="Q118" s="255"/>
+      <c r="R118" s="256"/>
+    </row>
+    <row r="119" spans="12:18" ht="23.4">
+      <c r="L119" s="255"/>
+      <c r="M119" s="255"/>
+      <c r="N119" s="255"/>
+      <c r="O119" s="255"/>
+      <c r="P119" s="255"/>
+      <c r="Q119" s="255"/>
+      <c r="R119" s="256"/>
+    </row>
+    <row r="120" spans="12:18" ht="23.4">
+      <c r="L120" s="255"/>
+      <c r="M120" s="255"/>
+      <c r="N120" s="255"/>
+      <c r="O120" s="255"/>
+      <c r="P120" s="255"/>
+      <c r="Q120" s="255"/>
+      <c r="R120" s="256"/>
+    </row>
+    <row r="121" spans="12:18" ht="23.4">
+      <c r="L121" s="255"/>
+      <c r="M121" s="255"/>
+      <c r="N121" s="255"/>
+      <c r="O121" s="255"/>
+      <c r="P121" s="255"/>
+      <c r="Q121" s="255"/>
+      <c r="R121" s="256"/>
+    </row>
+    <row r="122" spans="12:18" ht="23.4">
+      <c r="L122" s="255"/>
+      <c r="M122" s="255"/>
+      <c r="N122" s="255"/>
+      <c r="O122" s="255"/>
+      <c r="P122" s="255"/>
+      <c r="Q122" s="255"/>
+      <c r="R122" s="256"/>
+    </row>
+    <row r="123" spans="12:18" ht="23.4">
+      <c r="L123" s="255"/>
+      <c r="M123" s="255"/>
+      <c r="N123" s="255"/>
+      <c r="O123" s="255"/>
+      <c r="P123" s="255"/>
+      <c r="Q123" s="255"/>
+      <c r="R123" s="256"/>
+    </row>
+    <row r="124" spans="12:18" ht="23.4">
+      <c r="L124" s="255"/>
+      <c r="M124" s="255"/>
+      <c r="N124" s="255"/>
+      <c r="O124" s="255"/>
+      <c r="P124" s="255"/>
+      <c r="Q124" s="255"/>
+      <c r="R124" s="256"/>
+    </row>
+    <row r="125" spans="12:18" ht="23.4">
+      <c r="L125" s="255"/>
+      <c r="M125" s="255"/>
+      <c r="N125" s="255"/>
+      <c r="O125" s="255"/>
+      <c r="P125" s="255"/>
+      <c r="Q125" s="255"/>
+      <c r="R125" s="256"/>
+    </row>
+    <row r="126" spans="12:18" ht="23.4">
+      <c r="L126" s="255"/>
+      <c r="M126" s="255"/>
+      <c r="N126" s="255"/>
+      <c r="O126" s="255"/>
+      <c r="P126" s="255"/>
+      <c r="Q126" s="255"/>
+      <c r="R126" s="256"/>
+    </row>
+    <row r="127" spans="12:18" ht="23.4">
+      <c r="L127" s="255"/>
+      <c r="M127" s="255"/>
+      <c r="N127" s="255"/>
+      <c r="O127" s="255"/>
+      <c r="P127" s="255"/>
+      <c r="Q127" s="255"/>
+      <c r="R127" s="256"/>
+    </row>
+    <row r="128" spans="12:18" ht="23.4">
+      <c r="L128" s="255"/>
+      <c r="M128" s="255"/>
+      <c r="N128" s="255"/>
+      <c r="O128" s="255"/>
+      <c r="P128" s="255"/>
+      <c r="Q128" s="255"/>
+      <c r="R128" s="256"/>
+    </row>
+    <row r="129" spans="12:18" ht="23.4">
+      <c r="L129" s="255"/>
+      <c r="M129" s="255"/>
+      <c r="N129" s="255"/>
+      <c r="O129" s="255"/>
+      <c r="P129" s="255"/>
+      <c r="Q129" s="255"/>
+      <c r="R129" s="256"/>
+    </row>
+    <row r="130" spans="12:18" ht="23.4">
+      <c r="L130" s="255"/>
+      <c r="M130" s="255"/>
+      <c r="N130" s="255"/>
+      <c r="O130" s="255"/>
+      <c r="P130" s="255"/>
+      <c r="Q130" s="255"/>
+      <c r="R130" s="256"/>
+    </row>
+    <row r="131" spans="12:18" ht="23.4">
+      <c r="L131" s="255"/>
+      <c r="M131" s="255"/>
+      <c r="N131" s="255"/>
+      <c r="O131" s="255"/>
+      <c r="P131" s="255"/>
+      <c r="Q131" s="255"/>
+      <c r="R131" s="256"/>
+    </row>
+    <row r="132" spans="12:18" ht="23.4">
+      <c r="L132" s="255"/>
+      <c r="M132" s="255"/>
+      <c r="N132" s="255"/>
+      <c r="O132" s="255"/>
+      <c r="P132" s="255"/>
+      <c r="Q132" s="255"/>
+      <c r="R132" s="256"/>
+    </row>
+    <row r="133" spans="12:18" ht="23.4">
+      <c r="L133" s="255"/>
+      <c r="M133" s="255"/>
+      <c r="N133" s="255"/>
+      <c r="O133" s="255"/>
+      <c r="P133" s="255"/>
+      <c r="Q133" s="255"/>
+      <c r="R133" s="256"/>
+    </row>
+    <row r="134" spans="12:18" ht="23.4">
+      <c r="L134" s="255"/>
+      <c r="M134" s="255"/>
+      <c r="N134" s="255"/>
+      <c r="O134" s="255"/>
+      <c r="P134" s="255"/>
+      <c r="Q134" s="255"/>
+      <c r="R134" s="256"/>
+    </row>
+    <row r="135" spans="12:18" ht="23.4">
+      <c r="L135" s="255"/>
+      <c r="M135" s="255"/>
+      <c r="N135" s="255"/>
+      <c r="O135" s="255"/>
+      <c r="P135" s="255"/>
+      <c r="Q135" s="255"/>
+      <c r="R135" s="256"/>
+    </row>
+    <row r="136" spans="12:18" ht="23.4">
+      <c r="L136" s="255"/>
+      <c r="M136" s="255"/>
+      <c r="N136" s="255"/>
+      <c r="O136" s="255"/>
+      <c r="P136" s="255"/>
+      <c r="Q136" s="255"/>
+      <c r="R136" s="256"/>
+    </row>
+    <row r="137" spans="12:18" ht="23.4">
+      <c r="L137" s="255"/>
+      <c r="M137" s="255"/>
+      <c r="N137" s="255"/>
+      <c r="O137" s="255"/>
+      <c r="P137" s="255"/>
+      <c r="Q137" s="255"/>
+      <c r="R137" s="256"/>
+    </row>
+    <row r="138" spans="12:18" ht="23.4">
+      <c r="L138" s="255"/>
+      <c r="M138" s="255"/>
+      <c r="N138" s="255"/>
+      <c r="O138" s="255"/>
+      <c r="P138" s="255"/>
+      <c r="Q138" s="255"/>
+      <c r="R138" s="256"/>
+    </row>
+    <row r="139" spans="12:18" ht="23.4">
+      <c r="L139" s="255"/>
+      <c r="M139" s="255"/>
+      <c r="N139" s="255"/>
+      <c r="O139" s="255"/>
+      <c r="P139" s="255"/>
+      <c r="Q139" s="255"/>
+      <c r="R139" s="256"/>
+    </row>
+    <row r="140" spans="12:18" ht="23.4">
+      <c r="L140" s="255"/>
+      <c r="M140" s="255"/>
+      <c r="N140" s="255"/>
+      <c r="O140" s="255"/>
+      <c r="P140" s="255"/>
+      <c r="Q140" s="255"/>
+      <c r="R140" s="256"/>
+    </row>
+    <row r="141" spans="12:18" ht="23.4">
+      <c r="L141" s="255"/>
+      <c r="M141" s="255"/>
+      <c r="N141" s="255"/>
+      <c r="O141" s="255"/>
+      <c r="P141" s="255"/>
+      <c r="Q141" s="255"/>
+      <c r="R141" s="256"/>
+    </row>
+    <row r="142" spans="12:18" ht="23.4">
+      <c r="L142" s="255"/>
+      <c r="M142" s="255"/>
+      <c r="N142" s="255"/>
+      <c r="O142" s="255"/>
+      <c r="P142" s="255"/>
+      <c r="Q142" s="255"/>
+      <c r="R142" s="256"/>
+    </row>
+    <row r="143" spans="12:18" ht="23.4">
+      <c r="L143" s="255"/>
+      <c r="M143" s="255"/>
+      <c r="N143" s="255"/>
+      <c r="O143" s="255"/>
+      <c r="P143" s="255"/>
+      <c r="Q143" s="255"/>
+      <c r="R143" s="256"/>
+    </row>
+    <row r="144" spans="12:18" ht="23.4">
+      <c r="L144" s="255"/>
+      <c r="M144" s="255"/>
+      <c r="N144" s="255"/>
+      <c r="O144" s="255"/>
+      <c r="P144" s="255"/>
+      <c r="Q144" s="255"/>
+      <c r="R144" s="256"/>
+    </row>
+    <row r="145" spans="12:18" ht="23.4">
+      <c r="L145" s="255"/>
+      <c r="M145" s="255"/>
+      <c r="N145" s="255"/>
+      <c r="O145" s="255"/>
+      <c r="P145" s="255"/>
+      <c r="Q145" s="255"/>
+      <c r="R145" s="256"/>
+    </row>
+    <row r="146" spans="12:18" ht="23.4">
+      <c r="L146" s="255"/>
+      <c r="M146" s="255"/>
+      <c r="N146" s="255"/>
+      <c r="O146" s="255"/>
+      <c r="P146" s="255"/>
+      <c r="Q146" s="255"/>
+      <c r="R146" s="256"/>
+    </row>
+    <row r="147" spans="12:18" ht="23.4">
+      <c r="L147" s="255"/>
+      <c r="M147" s="255"/>
+      <c r="N147" s="255"/>
+      <c r="O147" s="255"/>
+      <c r="P147" s="255"/>
+      <c r="Q147" s="255"/>
+      <c r="R147" s="256"/>
+    </row>
+    <row r="148" spans="12:18" ht="23.4">
+      <c r="L148" s="255"/>
+      <c r="M148" s="255"/>
+      <c r="N148" s="255"/>
+      <c r="O148" s="255"/>
+      <c r="P148" s="255"/>
+      <c r="Q148" s="255"/>
+      <c r="R148" s="256"/>
+    </row>
+    <row r="149" spans="12:18" ht="23.4">
+      <c r="L149" s="255"/>
+      <c r="M149" s="255"/>
+      <c r="N149" s="255"/>
+      <c r="O149" s="255"/>
+      <c r="P149" s="255"/>
+      <c r="Q149" s="255"/>
+      <c r="R149" s="256"/>
+    </row>
+    <row r="150" spans="12:18" ht="23.4">
+      <c r="L150" s="255"/>
+      <c r="M150" s="255"/>
+      <c r="N150" s="255"/>
+      <c r="O150" s="255"/>
+      <c r="P150" s="255"/>
+      <c r="Q150" s="255"/>
+      <c r="R150" s="256"/>
+    </row>
+    <row r="151" spans="12:18" ht="23.4">
+      <c r="L151" s="255"/>
+      <c r="M151" s="255"/>
+      <c r="N151" s="255"/>
+      <c r="O151" s="255"/>
+      <c r="P151" s="255"/>
+      <c r="Q151" s="255"/>
+      <c r="R151" s="256"/>
+    </row>
+    <row r="152" spans="12:18" ht="23.4">
+      <c r="L152" s="255"/>
+      <c r="M152" s="255"/>
+      <c r="N152" s="255"/>
+      <c r="O152" s="255"/>
+      <c r="P152" s="255"/>
+      <c r="Q152" s="255"/>
+      <c r="R152" s="256"/>
+    </row>
+    <row r="153" spans="12:18" ht="23.4">
+      <c r="L153" s="255"/>
+      <c r="M153" s="255"/>
+      <c r="N153" s="255"/>
+      <c r="O153" s="255"/>
+      <c r="P153" s="255"/>
+      <c r="Q153" s="255"/>
+      <c r="R153" s="256"/>
+    </row>
+    <row r="154" spans="12:18" ht="23.4">
+      <c r="L154" s="255"/>
+      <c r="M154" s="255"/>
+      <c r="N154" s="255"/>
+      <c r="O154" s="255"/>
+      <c r="P154" s="255"/>
+      <c r="Q154" s="255"/>
+      <c r="R154" s="256"/>
+    </row>
+    <row r="155" spans="12:18" ht="23.4">
+      <c r="L155" s="255"/>
+      <c r="M155" s="255"/>
+      <c r="N155" s="255"/>
+      <c r="O155" s="255"/>
+      <c r="P155" s="255"/>
+      <c r="Q155" s="255"/>
+      <c r="R155" s="256"/>
+    </row>
+    <row r="156" spans="12:18" ht="23.4">
+      <c r="L156" s="255"/>
+      <c r="M156" s="255"/>
+      <c r="N156" s="255"/>
+      <c r="O156" s="255"/>
+      <c r="P156" s="255"/>
+      <c r="Q156" s="255"/>
+      <c r="R156" s="256"/>
+    </row>
+    <row r="157" spans="12:18" ht="23.4">
+      <c r="L157" s="255"/>
+      <c r="M157" s="255"/>
+      <c r="N157" s="255"/>
+      <c r="O157" s="255"/>
+      <c r="P157" s="255"/>
+      <c r="Q157" s="255"/>
+      <c r="R157" s="256"/>
+    </row>
+    <row r="158" spans="12:18" ht="23.4">
+      <c r="L158" s="255"/>
+      <c r="M158" s="255"/>
+      <c r="N158" s="255"/>
+      <c r="O158" s="255"/>
+      <c r="P158" s="255"/>
+      <c r="Q158" s="255"/>
+      <c r="R158" s="256"/>
+    </row>
+    <row r="159" spans="12:18" ht="23.4">
+      <c r="L159" s="255"/>
+      <c r="M159" s="255"/>
+      <c r="N159" s="255"/>
+      <c r="O159" s="255"/>
+      <c r="P159" s="255"/>
+      <c r="Q159" s="255"/>
+      <c r="R159" s="256"/>
+    </row>
+    <row r="160" spans="12:18" ht="23.4">
+      <c r="L160" s="255"/>
+      <c r="M160" s="255"/>
+      <c r="N160" s="255"/>
+      <c r="O160" s="255"/>
+      <c r="P160" s="255"/>
+      <c r="Q160" s="255"/>
+      <c r="R160" s="256"/>
+    </row>
+    <row r="161" spans="12:18" ht="23.4">
+      <c r="L161" s="255"/>
+      <c r="M161" s="255"/>
+      <c r="N161" s="255"/>
+      <c r="O161" s="255"/>
+      <c r="P161" s="255"/>
+      <c r="Q161" s="255"/>
+      <c r="R161" s="256"/>
+    </row>
+    <row r="162" spans="12:18" ht="23.4">
+      <c r="L162" s="255"/>
+      <c r="M162" s="255"/>
+      <c r="N162" s="255"/>
+      <c r="O162" s="255"/>
+      <c r="P162" s="255"/>
+      <c r="Q162" s="255"/>
+      <c r="R162" s="256"/>
+    </row>
+    <row r="163" spans="12:18" ht="23.4">
+      <c r="L163" s="255"/>
+      <c r="M163" s="255"/>
+      <c r="N163" s="255"/>
+      <c r="O163" s="255"/>
+      <c r="P163" s="255"/>
+      <c r="Q163" s="255"/>
+      <c r="R163" s="256"/>
+    </row>
+    <row r="164" spans="12:18" ht="23.4">
+      <c r="L164" s="255"/>
+      <c r="M164" s="255"/>
+      <c r="N164" s="255"/>
+      <c r="O164" s="255"/>
+      <c r="P164" s="255"/>
+      <c r="Q164" s="255"/>
+      <c r="R164" s="256"/>
+    </row>
+    <row r="165" spans="12:18" ht="23.4">
+      <c r="L165" s="255"/>
+      <c r="M165" s="255"/>
+      <c r="N165" s="255"/>
+      <c r="O165" s="255"/>
+      <c r="P165" s="255"/>
+      <c r="Q165" s="255"/>
+      <c r="R165" s="256"/>
+    </row>
+    <row r="166" spans="12:18" ht="23.4">
+      <c r="L166" s="255"/>
+      <c r="M166" s="255"/>
+      <c r="N166" s="255"/>
+      <c r="O166" s="255"/>
+      <c r="P166" s="255"/>
+      <c r="Q166" s="255"/>
+      <c r="R166" s="256"/>
+    </row>
+    <row r="167" spans="12:18" ht="23.4">
+      <c r="L167" s="255"/>
+      <c r="M167" s="255"/>
+      <c r="N167" s="255"/>
+      <c r="O167" s="255"/>
+      <c r="P167" s="255"/>
+      <c r="Q167" s="255"/>
+      <c r="R167" s="256"/>
+    </row>
+    <row r="168" spans="12:18" ht="23.4">
+      <c r="L168" s="255"/>
+      <c r="M168" s="255"/>
+      <c r="N168" s="255"/>
+      <c r="O168" s="255"/>
+      <c r="P168" s="255"/>
+      <c r="Q168" s="255"/>
+      <c r="R168" s="256"/>
+    </row>
+    <row r="169" spans="12:18" ht="23.4">
+      <c r="L169" s="255"/>
+      <c r="M169" s="255"/>
+      <c r="N169" s="255"/>
+      <c r="O169" s="255"/>
+      <c r="P169" s="255"/>
+      <c r="Q169" s="255"/>
+      <c r="R169" s="256"/>
+    </row>
+    <row r="170" spans="12:18" ht="23.4">
+      <c r="L170" s="255"/>
+      <c r="M170" s="255"/>
+      <c r="N170" s="255"/>
+      <c r="O170" s="255"/>
+      <c r="P170" s="255"/>
+      <c r="Q170" s="255"/>
+      <c r="R170" s="256"/>
+    </row>
+    <row r="171" spans="12:18" ht="23.4">
+      <c r="L171" s="255"/>
+      <c r="M171" s="255"/>
+      <c r="N171" s="255"/>
+      <c r="O171" s="255"/>
+      <c r="P171" s="255"/>
+      <c r="Q171" s="255"/>
+      <c r="R171" s="256"/>
+    </row>
+    <row r="172" spans="12:18" ht="23.4">
+      <c r="L172" s="255"/>
+      <c r="M172" s="255"/>
+      <c r="N172" s="255"/>
+      <c r="O172" s="255"/>
+      <c r="P172" s="255"/>
+      <c r="Q172" s="255"/>
+      <c r="R172" s="256"/>
+    </row>
+    <row r="173" spans="12:18" ht="23.4">
+      <c r="L173" s="255"/>
+      <c r="M173" s="255"/>
+      <c r="N173" s="255"/>
+      <c r="O173" s="255"/>
+      <c r="P173" s="255"/>
+      <c r="Q173" s="255"/>
+      <c r="R173" s="256"/>
+    </row>
+    <row r="174" spans="12:18" ht="23.4">
+      <c r="L174" s="255"/>
+      <c r="M174" s="255"/>
+      <c r="N174" s="255"/>
+      <c r="O174" s="255"/>
+      <c r="P174" s="255"/>
+      <c r="Q174" s="255"/>
+      <c r="R174" s="256"/>
+    </row>
+    <row r="175" spans="12:18" ht="23.4">
+      <c r="L175" s="255"/>
+      <c r="M175" s="255"/>
+      <c r="N175" s="255"/>
+      <c r="O175" s="255"/>
+      <c r="P175" s="255"/>
+      <c r="Q175" s="255"/>
+      <c r="R175" s="256"/>
+    </row>
+    <row r="176" spans="12:18" ht="23.4">
+      <c r="L176" s="255"/>
+      <c r="M176" s="255"/>
+      <c r="N176" s="255"/>
+      <c r="O176" s="255"/>
+      <c r="P176" s="255"/>
+      <c r="Q176" s="255"/>
+      <c r="R176" s="256"/>
+    </row>
+    <row r="177" spans="12:18" ht="23.4">
+      <c r="L177" s="255"/>
+      <c r="M177" s="255"/>
+      <c r="N177" s="255"/>
+      <c r="O177" s="255"/>
+      <c r="P177" s="255"/>
+      <c r="Q177" s="255"/>
+      <c r="R177" s="256"/>
+    </row>
+    <row r="178" spans="12:18" ht="23.4">
+      <c r="L178" s="255"/>
+      <c r="M178" s="255"/>
+      <c r="N178" s="255"/>
+      <c r="O178" s="255"/>
+      <c r="P178" s="255"/>
+      <c r="Q178" s="255"/>
+      <c r="R178" s="256"/>
+    </row>
+    <row r="179" spans="12:18" ht="23.4">
+      <c r="L179" s="255"/>
+      <c r="M179" s="255"/>
+      <c r="N179" s="255"/>
+      <c r="O179" s="255"/>
+      <c r="P179" s="255"/>
+      <c r="Q179" s="255"/>
+      <c r="R179" s="256"/>
+    </row>
+    <row r="180" spans="12:18" ht="23.4">
+      <c r="L180" s="255"/>
+      <c r="M180" s="255"/>
+      <c r="N180" s="255"/>
+      <c r="O180" s="255"/>
+      <c r="P180" s="255"/>
+      <c r="Q180" s="255"/>
+      <c r="R180" s="256"/>
+    </row>
+    <row r="181" spans="12:18" ht="23.4">
+      <c r="L181" s="255"/>
+      <c r="M181" s="255"/>
+      <c r="N181" s="255"/>
+      <c r="O181" s="255"/>
+      <c r="P181" s="255"/>
+      <c r="Q181" s="255"/>
+      <c r="R181" s="256"/>
+    </row>
+    <row r="182" spans="12:18" ht="23.4">
+      <c r="L182" s="255"/>
+      <c r="M182" s="255"/>
+      <c r="N182" s="255"/>
+      <c r="O182" s="255"/>
+      <c r="P182" s="255"/>
+      <c r="Q182" s="255"/>
+      <c r="R182" s="256"/>
+    </row>
+    <row r="183" spans="12:18" ht="23.4">
+      <c r="L183" s="255"/>
+      <c r="M183" s="255"/>
+      <c r="N183" s="255"/>
+      <c r="O183" s="255"/>
+      <c r="P183" s="255"/>
+      <c r="Q183" s="255"/>
+      <c r="R183" s="256"/>
+    </row>
+    <row r="184" spans="12:18" ht="23.4">
+      <c r="L184" s="255"/>
+      <c r="M184" s="255"/>
+      <c r="N184" s="255"/>
+      <c r="O184" s="255"/>
+      <c r="P184" s="255"/>
+      <c r="Q184" s="255"/>
+      <c r="R184" s="256"/>
+    </row>
+    <row r="185" spans="12:18" ht="23.4">
+      <c r="L185" s="255"/>
+      <c r="M185" s="255"/>
+      <c r="N185" s="255"/>
+      <c r="O185" s="255"/>
+      <c r="P185" s="255"/>
+      <c r="Q185" s="255"/>
+      <c r="R185" s="256"/>
+    </row>
+    <row r="186" spans="12:18" ht="23.4">
+      <c r="L186" s="255"/>
+      <c r="M186" s="255"/>
+      <c r="N186" s="255"/>
+      <c r="O186" s="255"/>
+      <c r="P186" s="255"/>
+      <c r="Q186" s="255"/>
+      <c r="R186" s="256"/>
+    </row>
+    <row r="187" spans="12:18" ht="23.4">
+      <c r="L187" s="255"/>
+      <c r="M187" s="255"/>
+      <c r="N187" s="255"/>
+      <c r="O187" s="255"/>
+      <c r="P187" s="255"/>
+      <c r="Q187" s="255"/>
+      <c r="R187" s="256"/>
+    </row>
+    <row r="188" spans="12:18" ht="23.4">
+      <c r="L188" s="255"/>
+      <c r="M188" s="255"/>
+      <c r="N188" s="255"/>
+      <c r="O188" s="255"/>
+      <c r="P188" s="255"/>
+      <c r="Q188" s="255"/>
+      <c r="R188" s="256"/>
+    </row>
+    <row r="189" spans="12:18" ht="23.4">
+      <c r="L189" s="255"/>
+      <c r="M189" s="255"/>
+      <c r="N189" s="255"/>
+      <c r="O189" s="255"/>
+      <c r="P189" s="255"/>
+      <c r="Q189" s="255"/>
+      <c r="R189" s="256"/>
+    </row>
+    <row r="190" spans="12:18" ht="23.4">
+      <c r="L190" s="255"/>
+      <c r="M190" s="255"/>
+      <c r="N190" s="255"/>
+      <c r="O190" s="255"/>
+      <c r="P190" s="255"/>
+      <c r="Q190" s="255"/>
+      <c r="R190" s="256"/>
+    </row>
+    <row r="191" spans="12:18" ht="23.4">
+      <c r="L191" s="255"/>
+      <c r="M191" s="255"/>
+      <c r="N191" s="255"/>
+      <c r="O191" s="255"/>
+      <c r="P191" s="255"/>
+      <c r="Q191" s="255"/>
+      <c r="R191" s="256"/>
+    </row>
+    <row r="192" spans="12:18" ht="23.4">
+      <c r="L192" s="255"/>
+      <c r="M192" s="255"/>
+      <c r="N192" s="255"/>
+      <c r="O192" s="255"/>
+      <c r="P192" s="255"/>
+      <c r="Q192" s="255"/>
+      <c r="R192" s="256"/>
+    </row>
+    <row r="193" spans="12:18" ht="23.4">
+      <c r="L193" s="255"/>
+      <c r="M193" s="255"/>
+      <c r="N193" s="255"/>
+      <c r="O193" s="255"/>
+      <c r="P193" s="255"/>
+      <c r="Q193" s="255"/>
+      <c r="R193" s="256"/>
+    </row>
+    <row r="194" spans="12:18" ht="23.4">
+      <c r="L194" s="255"/>
+      <c r="M194" s="255"/>
+      <c r="N194" s="255"/>
+      <c r="O194" s="255"/>
+      <c r="P194" s="255"/>
+      <c r="Q194" s="255"/>
+      <c r="R194" s="256"/>
+    </row>
+    <row r="195" spans="12:18" ht="23.4">
+      <c r="L195" s="255"/>
+      <c r="M195" s="255"/>
+      <c r="N195" s="255"/>
+      <c r="O195" s="255"/>
+      <c r="P195" s="255"/>
+      <c r="Q195" s="255"/>
+      <c r="R195" s="256"/>
+    </row>
+    <row r="196" spans="12:18" ht="23.4">
+      <c r="L196" s="255"/>
+      <c r="M196" s="255"/>
+      <c r="N196" s="255"/>
+      <c r="O196" s="255"/>
+      <c r="P196" s="255"/>
+      <c r="Q196" s="255"/>
+      <c r="R196" s="256"/>
+    </row>
+    <row r="197" spans="12:18" ht="23.4">
+      <c r="L197" s="255"/>
+      <c r="M197" s="255"/>
+      <c r="N197" s="255"/>
+      <c r="O197" s="255"/>
+      <c r="P197" s="255"/>
+      <c r="Q197" s="255"/>
+      <c r="R197" s="256"/>
+    </row>
+    <row r="198" spans="12:18" ht="23.4">
+      <c r="L198" s="255"/>
+      <c r="M198" s="255"/>
+      <c r="N198" s="255"/>
+      <c r="O198" s="255"/>
+      <c r="P198" s="255"/>
+      <c r="Q198" s="255"/>
+      <c r="R198" s="256"/>
+    </row>
+    <row r="199" spans="12:18" ht="23.4">
+      <c r="L199" s="255"/>
+      <c r="M199" s="255"/>
+      <c r="N199" s="255"/>
+      <c r="O199" s="255"/>
+      <c r="P199" s="255"/>
+      <c r="Q199" s="255"/>
+      <c r="R199" s="256"/>
+    </row>
+    <row r="200" spans="12:18" ht="23.4">
+      <c r="L200" s="255"/>
+      <c r="M200" s="255"/>
+      <c r="N200" s="255"/>
+      <c r="O200" s="255"/>
+      <c r="P200" s="255"/>
+      <c r="Q200" s="255"/>
+      <c r="R200" s="256"/>
+    </row>
+    <row r="201" spans="12:18" ht="23.4">
+      <c r="L201" s="255"/>
+      <c r="M201" s="255"/>
+      <c r="N201" s="255"/>
+      <c r="O201" s="255"/>
+      <c r="P201" s="255"/>
+      <c r="Q201" s="255"/>
+      <c r="R201" s="256"/>
+    </row>
+    <row r="202" spans="12:18" ht="23.4">
+      <c r="L202" s="255"/>
+      <c r="M202" s="255"/>
+      <c r="N202" s="255"/>
+      <c r="O202" s="255"/>
+      <c r="P202" s="255"/>
+      <c r="Q202" s="255"/>
+      <c r="R202" s="256"/>
+    </row>
+    <row r="203" spans="12:18" ht="23.4">
+      <c r="L203" s="255"/>
+      <c r="M203" s="255"/>
+      <c r="N203" s="255"/>
+      <c r="O203" s="255"/>
+      <c r="P203" s="255"/>
+      <c r="Q203" s="255"/>
+      <c r="R203" s="256"/>
+    </row>
+    <row r="204" spans="12:18" ht="23.4">
+      <c r="L204" s="255"/>
+      <c r="M204" s="255"/>
+      <c r="N204" s="255"/>
+      <c r="O204" s="255"/>
+      <c r="P204" s="255"/>
+      <c r="Q204" s="255"/>
+      <c r="R204" s="256"/>
+    </row>
+    <row r="205" spans="12:18" ht="23.4">
+      <c r="L205" s="255"/>
+      <c r="M205" s="255"/>
+      <c r="N205" s="255"/>
+      <c r="O205" s="255"/>
+      <c r="P205" s="255"/>
+      <c r="Q205" s="255"/>
+      <c r="R205" s="256"/>
+    </row>
+    <row r="206" spans="12:18" ht="23.4">
+      <c r="L206" s="255"/>
+      <c r="M206" s="255"/>
+      <c r="N206" s="255"/>
+      <c r="O206" s="255"/>
+      <c r="P206" s="255"/>
+      <c r="Q206" s="255"/>
+      <c r="R206" s="256"/>
+    </row>
+    <row r="207" spans="12:18" ht="23.4">
+      <c r="L207" s="255"/>
+      <c r="M207" s="255"/>
+      <c r="N207" s="255"/>
+      <c r="O207" s="255"/>
+      <c r="P207" s="255"/>
+      <c r="Q207" s="255"/>
+      <c r="R207" s="256"/>
+    </row>
+    <row r="208" spans="12:18" ht="23.4">
+      <c r="L208" s="255"/>
+      <c r="M208" s="255"/>
+      <c r="N208" s="255"/>
+      <c r="O208" s="255"/>
+      <c r="P208" s="255"/>
+      <c r="Q208" s="255"/>
+      <c r="R208" s="256"/>
+    </row>
+    <row r="209" spans="12:18" ht="23.4">
+      <c r="L209" s="255"/>
+      <c r="M209" s="255"/>
+      <c r="N209" s="255"/>
+      <c r="O209" s="255"/>
+      <c r="P209" s="255"/>
+      <c r="Q209" s="255"/>
+      <c r="R209" s="256"/>
+    </row>
+    <row r="210" spans="12:18" ht="23.4">
+      <c r="L210" s="255"/>
+      <c r="M210" s="255"/>
+      <c r="N210" s="255"/>
+      <c r="O210" s="255"/>
+      <c r="P210" s="255"/>
+      <c r="Q210" s="255"/>
+      <c r="R210" s="256"/>
+    </row>
+    <row r="211" spans="12:18" ht="23.4">
+      <c r="L211" s="255"/>
+      <c r="M211" s="255"/>
+      <c r="N211" s="255"/>
+      <c r="O211" s="255"/>
+      <c r="P211" s="255"/>
+      <c r="Q211" s="255"/>
+      <c r="R211" s="256"/>
+    </row>
+    <row r="212" spans="12:18" ht="23.4">
+      <c r="L212" s="255"/>
+      <c r="M212" s="255"/>
+      <c r="N212" s="255"/>
+      <c r="O212" s="255"/>
+      <c r="P212" s="255"/>
+      <c r="Q212" s="255"/>
+      <c r="R212" s="256"/>
+    </row>
+    <row r="213" spans="12:18" ht="23.4">
+      <c r="L213" s="255"/>
+      <c r="M213" s="255"/>
+      <c r="N213" s="255"/>
+      <c r="O213" s="255"/>
+      <c r="P213" s="255"/>
+      <c r="Q213" s="255"/>
+      <c r="R213" s="256"/>
+    </row>
+    <row r="214" spans="12:18" ht="23.4">
+      <c r="L214" s="255"/>
+      <c r="M214" s="255"/>
+      <c r="N214" s="255"/>
+      <c r="O214" s="255"/>
+      <c r="P214" s="255"/>
+      <c r="Q214" s="255"/>
+      <c r="R214" s="256"/>
+    </row>
+    <row r="215" spans="12:18" ht="23.4">
+      <c r="L215" s="255"/>
+      <c r="M215" s="255"/>
+      <c r="N215" s="255"/>
+      <c r="O215" s="255"/>
+      <c r="P215" s="255"/>
+      <c r="Q215" s="255"/>
+      <c r="R215" s="256"/>
+    </row>
+    <row r="216" spans="12:18" ht="23.4">
+      <c r="L216" s="255"/>
+      <c r="M216" s="255"/>
+      <c r="N216" s="255"/>
+      <c r="O216" s="255"/>
+      <c r="P216" s="255"/>
+      <c r="Q216" s="255"/>
+      <c r="R216" s="256"/>
+    </row>
+    <row r="217" spans="12:18" ht="23.4">
+      <c r="L217" s="255"/>
+      <c r="M217" s="255"/>
+      <c r="N217" s="255"/>
+      <c r="O217" s="255"/>
+      <c r="P217" s="255"/>
+      <c r="Q217" s="255"/>
+      <c r="R217" s="256"/>
+    </row>
+    <row r="218" spans="12:18" ht="23.4">
+      <c r="L218" s="255"/>
+      <c r="M218" s="255"/>
+      <c r="N218" s="255"/>
+      <c r="O218" s="255"/>
+      <c r="P218" s="255"/>
+      <c r="Q218" s="255"/>
+      <c r="R218" s="256"/>
+    </row>
+    <row r="219" spans="12:18" ht="23.4">
+      <c r="L219" s="255"/>
+      <c r="M219" s="255"/>
+      <c r="N219" s="255"/>
+      <c r="O219" s="255"/>
+      <c r="P219" s="255"/>
+      <c r="Q219" s="255"/>
+      <c r="R219" s="256"/>
+    </row>
+    <row r="220" spans="12:18" ht="23.4">
+      <c r="L220" s="255"/>
+      <c r="M220" s="255"/>
+      <c r="N220" s="255"/>
+      <c r="O220" s="255"/>
+      <c r="P220" s="255"/>
+      <c r="Q220" s="255"/>
+      <c r="R220" s="256"/>
+    </row>
+    <row r="221" spans="12:18" ht="23.4">
+      <c r="L221" s="255"/>
+      <c r="M221" s="255"/>
+      <c r="N221" s="255"/>
+      <c r="O221" s="255"/>
+      <c r="P221" s="255"/>
+      <c r="Q221" s="255"/>
+      <c r="R221" s="256"/>
+    </row>
+    <row r="222" spans="12:18" ht="23.4">
+      <c r="L222" s="255"/>
+      <c r="M222" s="255"/>
+      <c r="N222" s="255"/>
+      <c r="O222" s="255"/>
+      <c r="P222" s="255"/>
+      <c r="Q222" s="255"/>
+      <c r="R222" s="256"/>
+    </row>
+    <row r="223" spans="12:18" ht="23.4">
+      <c r="L223" s="255"/>
+      <c r="M223" s="255"/>
+      <c r="N223" s="255"/>
+      <c r="O223" s="255"/>
+      <c r="P223" s="255"/>
+      <c r="Q223" s="255"/>
+      <c r="R223" s="256"/>
+    </row>
+    <row r="224" spans="12:18" ht="23.4">
+      <c r="L224" s="255"/>
+      <c r="M224" s="255"/>
+      <c r="N224" s="255"/>
+      <c r="O224" s="255"/>
+      <c r="P224" s="255"/>
+      <c r="Q224" s="255"/>
+      <c r="R224" s="256"/>
+    </row>
+    <row r="225" spans="12:18" ht="23.4">
+      <c r="L225" s="255"/>
+      <c r="M225" s="255"/>
+      <c r="N225" s="255"/>
+      <c r="O225" s="255"/>
+      <c r="P225" s="255"/>
+      <c r="Q225" s="255"/>
+      <c r="R225" s="256"/>
+    </row>
+    <row r="226" spans="12:18" ht="23.4">
+      <c r="L226" s="255"/>
+      <c r="M226" s="255"/>
+      <c r="N226" s="255"/>
+      <c r="O226" s="255"/>
+      <c r="P226" s="255"/>
+      <c r="Q226" s="255"/>
+      <c r="R226" s="256"/>
+    </row>
+    <row r="227" spans="12:18" ht="23.4">
+      <c r="L227" s="255"/>
+      <c r="M227" s="255"/>
+      <c r="N227" s="255"/>
+      <c r="O227" s="255"/>
+      <c r="P227" s="255"/>
+      <c r="Q227" s="255"/>
+      <c r="R227" s="256"/>
+    </row>
+    <row r="228" spans="12:18" ht="23.4">
+      <c r="L228" s="255"/>
+      <c r="M228" s="255"/>
+      <c r="N228" s="255"/>
+      <c r="O228" s="255"/>
+      <c r="P228" s="255"/>
+      <c r="Q228" s="255"/>
+      <c r="R228" s="256"/>
+    </row>
+    <row r="229" spans="12:18" ht="23.4">
+      <c r="L229" s="255"/>
+      <c r="M229" s="255"/>
+      <c r="N229" s="255"/>
+      <c r="O229" s="255"/>
+      <c r="P229" s="255"/>
+      <c r="Q229" s="255"/>
+      <c r="R229" s="256"/>
+    </row>
+    <row r="230" spans="12:18" ht="23.4">
+      <c r="L230" s="255"/>
+      <c r="M230" s="255"/>
+      <c r="N230" s="255"/>
+      <c r="O230" s="255"/>
+      <c r="P230" s="255"/>
+      <c r="Q230" s="255"/>
+      <c r="R230" s="256"/>
+    </row>
+    <row r="231" spans="12:18" ht="23.4">
+      <c r="L231" s="255"/>
+      <c r="M231" s="255"/>
+      <c r="N231" s="255"/>
+      <c r="O231" s="255"/>
+      <c r="P231" s="255"/>
+      <c r="Q231" s="255"/>
+      <c r="R231" s="256"/>
+    </row>
+    <row r="232" spans="12:18" ht="23.4">
+      <c r="L232" s="255"/>
+      <c r="M232" s="255"/>
+      <c r="N232" s="255"/>
+      <c r="O232" s="255"/>
+      <c r="P232" s="255"/>
+      <c r="Q232" s="255"/>
+      <c r="R232" s="256"/>
+    </row>
+    <row r="233" spans="12:18" ht="23.4">
+      <c r="L233" s="255"/>
+      <c r="M233" s="255"/>
+      <c r="N233" s="255"/>
+      <c r="O233" s="255"/>
+      <c r="P233" s="255"/>
+      <c r="Q233" s="255"/>
+      <c r="R233" s="256"/>
+    </row>
+    <row r="234" spans="12:18" ht="23.4">
+      <c r="L234" s="255"/>
+      <c r="M234" s="255"/>
+      <c r="N234" s="255"/>
+      <c r="O234" s="255"/>
+      <c r="P234" s="255"/>
+      <c r="Q234" s="255"/>
+      <c r="R234" s="256"/>
+    </row>
+    <row r="235" spans="12:18" ht="23.4">
+      <c r="L235" s="255"/>
+      <c r="M235" s="255"/>
+      <c r="N235" s="255"/>
+      <c r="O235" s="255"/>
+      <c r="P235" s="255"/>
+      <c r="Q235" s="255"/>
+      <c r="R235" s="256"/>
+    </row>
+    <row r="236" spans="12:18" ht="23.4">
+      <c r="L236" s="255"/>
+      <c r="M236" s="255"/>
+      <c r="N236" s="255"/>
+      <c r="O236" s="255"/>
+      <c r="P236" s="255"/>
+      <c r="Q236" s="255"/>
+      <c r="R236" s="256"/>
+    </row>
+    <row r="237" spans="12:18" ht="23.4">
+      <c r="L237" s="255"/>
+      <c r="M237" s="255"/>
+      <c r="N237" s="255"/>
+      <c r="O237" s="255"/>
+      <c r="P237" s="255"/>
+      <c r="Q237" s="255"/>
+      <c r="R237" s="256"/>
+    </row>
+    <row r="238" spans="12:18" ht="23.4">
+      <c r="L238" s="255"/>
+      <c r="M238" s="255"/>
+      <c r="N238" s="255"/>
+      <c r="O238" s="255"/>
+      <c r="P238" s="255"/>
+      <c r="Q238" s="255"/>
+      <c r="R238" s="256"/>
+    </row>
+    <row r="239" spans="12:18" ht="23.4">
+      <c r="L239" s="255"/>
+      <c r="M239" s="255"/>
+      <c r="N239" s="255"/>
+      <c r="O239" s="255"/>
+      <c r="P239" s="255"/>
+      <c r="Q239" s="255"/>
+      <c r="R239" s="256"/>
+    </row>
+    <row r="240" spans="12:18" ht="23.4">
+      <c r="L240" s="255"/>
+      <c r="M240" s="255"/>
+      <c r="N240" s="255"/>
+      <c r="O240" s="255"/>
+      <c r="P240" s="255"/>
+      <c r="Q240" s="255"/>
+      <c r="R240" s="256"/>
+    </row>
+    <row r="241" spans="12:18" ht="23.4">
+      <c r="L241" s="255"/>
+      <c r="M241" s="255"/>
+      <c r="N241" s="255"/>
+      <c r="O241" s="255"/>
+      <c r="P241" s="255"/>
+      <c r="Q241" s="255"/>
+      <c r="R241" s="256"/>
+    </row>
+    <row r="242" spans="12:18" ht="23.4">
+      <c r="L242" s="255"/>
+      <c r="M242" s="255"/>
+      <c r="N242" s="255"/>
+      <c r="O242" s="255"/>
+      <c r="P242" s="255"/>
+      <c r="Q242" s="255"/>
+      <c r="R242" s="256"/>
+    </row>
+    <row r="243" spans="12:18" ht="23.4">
+      <c r="L243" s="255"/>
+      <c r="M243" s="255"/>
+      <c r="N243" s="255"/>
+      <c r="O243" s="255"/>
+      <c r="P243" s="255"/>
+      <c r="Q243" s="255"/>
+      <c r="R243" s="256"/>
+    </row>
+    <row r="244" spans="12:18" ht="23.4">
+      <c r="L244" s="255"/>
+      <c r="M244" s="255"/>
+      <c r="N244" s="255"/>
+      <c r="O244" s="255"/>
+      <c r="P244" s="255"/>
+      <c r="Q244" s="255"/>
+      <c r="R244" s="256"/>
+    </row>
+    <row r="245" spans="12:18" ht="23.4">
+      <c r="L245" s="255"/>
+      <c r="M245" s="255"/>
+      <c r="N245" s="255"/>
+      <c r="O245" s="255"/>
+      <c r="P245" s="255"/>
+      <c r="Q245" s="255"/>
+      <c r="R245" s="256"/>
+    </row>
+    <row r="246" spans="12:18" ht="23.4">
+      <c r="L246" s="255"/>
+      <c r="M246" s="255"/>
+      <c r="N246" s="255"/>
+      <c r="O246" s="255"/>
+      <c r="P246" s="255"/>
+      <c r="Q246" s="255"/>
+      <c r="R246" s="256"/>
+    </row>
+    <row r="247" spans="12:18" ht="23.4">
+      <c r="L247" s="255"/>
+      <c r="M247" s="255"/>
+      <c r="N247" s="255"/>
+      <c r="O247" s="255"/>
+      <c r="P247" s="255"/>
+      <c r="Q247" s="255"/>
+      <c r="R247" s="256"/>
+    </row>
+    <row r="248" spans="12:18" ht="23.4">
+      <c r="L248" s="255"/>
+      <c r="M248" s="255"/>
+      <c r="N248" s="255"/>
+      <c r="O248" s="255"/>
+      <c r="P248" s="255"/>
+      <c r="Q248" s="255"/>
+      <c r="R248" s="256"/>
+    </row>
+    <row r="249" spans="12:18" ht="23.4">
+      <c r="L249" s="255"/>
+      <c r="M249" s="255"/>
+      <c r="N249" s="255"/>
+      <c r="O249" s="255"/>
+      <c r="P249" s="255"/>
+      <c r="Q249" s="255"/>
+      <c r="R249" s="256"/>
+    </row>
+    <row r="250" spans="12:18" ht="23.4">
+      <c r="L250" s="255"/>
+      <c r="M250" s="255"/>
+      <c r="N250" s="255"/>
+      <c r="O250" s="255"/>
+      <c r="P250" s="255"/>
+      <c r="Q250" s="255"/>
+      <c r="R250" s="256"/>
+    </row>
+    <row r="251" spans="12:18" ht="23.4">
+      <c r="L251" s="255"/>
+      <c r="M251" s="255"/>
+      <c r="N251" s="255"/>
+      <c r="O251" s="255"/>
+      <c r="P251" s="255"/>
+      <c r="Q251" s="255"/>
+      <c r="R251" s="256"/>
+    </row>
+    <row r="252" spans="12:18" ht="23.4">
+      <c r="L252" s="255"/>
+      <c r="M252" s="255"/>
+      <c r="N252" s="255"/>
+      <c r="O252" s="255"/>
+      <c r="P252" s="255"/>
+      <c r="Q252" s="255"/>
+      <c r="R252" s="256"/>
+    </row>
+    <row r="253" spans="12:18" ht="23.4">
+      <c r="L253" s="255"/>
+      <c r="M253" s="255"/>
+      <c r="N253" s="255"/>
+      <c r="O253" s="255"/>
+      <c r="P253" s="255"/>
+      <c r="Q253" s="255"/>
+      <c r="R253" s="256"/>
+    </row>
+    <row r="254" spans="12:18" ht="23.4">
+      <c r="L254" s="255"/>
+      <c r="M254" s="255"/>
+      <c r="N254" s="255"/>
+      <c r="O254" s="255"/>
+      <c r="P254" s="255"/>
+      <c r="Q254" s="255"/>
+      <c r="R254" s="256"/>
+    </row>
+    <row r="255" spans="12:18" ht="23.4">
+      <c r="L255" s="255"/>
+      <c r="M255" s="255"/>
+      <c r="N255" s="255"/>
+      <c r="O255" s="255"/>
+      <c r="P255" s="255"/>
+      <c r="Q255" s="255"/>
+      <c r="R255" s="256"/>
+    </row>
+    <row r="256" spans="12:18" ht="23.4">
+      <c r="L256" s="255"/>
+      <c r="M256" s="255"/>
+      <c r="N256" s="255"/>
+      <c r="O256" s="255"/>
+      <c r="P256" s="255"/>
+      <c r="Q256" s="255"/>
+      <c r="R256" s="256"/>
+    </row>
+    <row r="257" spans="12:18" ht="23.4">
+      <c r="L257" s="255"/>
+      <c r="M257" s="255"/>
+      <c r="N257" s="255"/>
+      <c r="O257" s="255"/>
+      <c r="P257" s="255"/>
+      <c r="Q257" s="255"/>
+      <c r="R257" s="256"/>
+    </row>
+    <row r="258" spans="12:18" ht="23.4">
+      <c r="L258" s="255"/>
+      <c r="M258" s="255"/>
+      <c r="N258" s="255"/>
+      <c r="O258" s="255"/>
+      <c r="P258" s="255"/>
+      <c r="Q258" s="255"/>
+      <c r="R258" s="256"/>
+    </row>
+    <row r="259" spans="12:18" ht="23.4">
+      <c r="L259" s="255"/>
+      <c r="M259" s="255"/>
+      <c r="N259" s="255"/>
+      <c r="O259" s="255"/>
+      <c r="P259" s="255"/>
+      <c r="Q259" s="255"/>
+      <c r="R259" s="256"/>
+    </row>
+    <row r="260" spans="12:18" ht="23.4">
+      <c r="L260" s="255"/>
+      <c r="M260" s="255"/>
+      <c r="N260" s="255"/>
+      <c r="O260" s="255"/>
+      <c r="P260" s="255"/>
+      <c r="Q260" s="255"/>
+      <c r="R260" s="256"/>
+    </row>
+    <row r="261" spans="12:18" ht="23.4">
+      <c r="L261" s="255"/>
+      <c r="M261" s="255"/>
+      <c r="N261" s="255"/>
+      <c r="O261" s="255"/>
+      <c r="P261" s="255"/>
+      <c r="Q261" s="255"/>
+      <c r="R261" s="256"/>
+    </row>
+    <row r="262" spans="12:18" ht="23.4">
+      <c r="L262" s="255"/>
+      <c r="M262" s="255"/>
+      <c r="N262" s="255"/>
+      <c r="O262" s="255"/>
+      <c r="P262" s="255"/>
+      <c r="Q262" s="255"/>
+      <c r="R262" s="256"/>
+    </row>
+    <row r="263" spans="12:18" ht="23.4">
+      <c r="L263" s="255"/>
+      <c r="M263" s="255"/>
+      <c r="N263" s="255"/>
+      <c r="O263" s="255"/>
+      <c r="P263" s="255"/>
+      <c r="Q263" s="255"/>
+      <c r="R263" s="256"/>
+    </row>
+    <row r="264" spans="12:18" ht="23.4">
+      <c r="L264" s="255"/>
+      <c r="M264" s="255"/>
+      <c r="N264" s="255"/>
+      <c r="O264" s="255"/>
+      <c r="P264" s="255"/>
+      <c r="Q264" s="255"/>
+      <c r="R264" s="256"/>
+    </row>
+    <row r="265" spans="12:18" ht="23.4">
+      <c r="L265" s="255"/>
+      <c r="M265" s="255"/>
+      <c r="N265" s="255"/>
+      <c r="O265" s="255"/>
+      <c r="P265" s="255"/>
+      <c r="Q265" s="255"/>
+      <c r="R265" s="256"/>
+    </row>
+    <row r="266" spans="12:18" ht="23.4">
+      <c r="L266" s="255"/>
+      <c r="M266" s="255"/>
+      <c r="N266" s="255"/>
+      <c r="O266" s="255"/>
+      <c r="P266" s="255"/>
+      <c r="Q266" s="255"/>
+      <c r="R266" s="256"/>
+    </row>
+    <row r="267" spans="12:18" ht="23.4">
+      <c r="L267" s="255"/>
+      <c r="M267" s="255"/>
+      <c r="N267" s="255"/>
+      <c r="O267" s="255"/>
+      <c r="P267" s="255"/>
+      <c r="Q267" s="255"/>
+      <c r="R267" s="256"/>
+    </row>
+    <row r="268" spans="12:18" ht="23.4">
+      <c r="L268" s="255"/>
+      <c r="M268" s="255"/>
+      <c r="N268" s="255"/>
+      <c r="O268" s="255"/>
+      <c r="P268" s="255"/>
+      <c r="Q268" s="255"/>
+      <c r="R268" s="256"/>
+    </row>
+    <row r="269" spans="12:18" ht="23.4">
+      <c r="L269" s="255"/>
+      <c r="M269" s="255"/>
+      <c r="N269" s="255"/>
+      <c r="O269" s="255"/>
+      <c r="P269" s="255"/>
+      <c r="Q269" s="255"/>
+      <c r="R269" s="256"/>
+    </row>
+    <row r="270" spans="12:18" ht="23.4">
+      <c r="L270" s="255"/>
+      <c r="M270" s="255"/>
+      <c r="N270" s="255"/>
+      <c r="O270" s="255"/>
+      <c r="P270" s="255"/>
+      <c r="Q270" s="255"/>
+      <c r="R270" s="256"/>
+    </row>
+    <row r="271" spans="12:18" ht="23.4">
+      <c r="L271" s="255"/>
+      <c r="M271" s="255"/>
+      <c r="N271" s="255"/>
+      <c r="O271" s="255"/>
+      <c r="P271" s="255"/>
+      <c r="Q271" s="255"/>
+      <c r="R271" s="256"/>
+    </row>
+    <row r="272" spans="12:18" ht="23.4">
+      <c r="L272" s="255"/>
+      <c r="M272" s="255"/>
+      <c r="N272" s="255"/>
+      <c r="O272" s="255"/>
+      <c r="P272" s="255"/>
+      <c r="Q272" s="255"/>
+      <c r="R272" s="256"/>
+    </row>
+    <row r="273" spans="12:18" ht="23.4">
+      <c r="L273" s="255"/>
+      <c r="M273" s="255"/>
+      <c r="N273" s="255"/>
+      <c r="O273" s="255"/>
+      <c r="P273" s="255"/>
+      <c r="Q273" s="255"/>
+      <c r="R273" s="256"/>
+    </row>
+    <row r="274" spans="12:18" ht="23.4">
+      <c r="L274" s="255"/>
+      <c r="M274" s="255"/>
+      <c r="N274" s="255"/>
+      <c r="O274" s="255"/>
+      <c r="P274" s="255"/>
+      <c r="Q274" s="255"/>
+      <c r="R274" s="256"/>
+    </row>
+    <row r="275" spans="12:18" ht="23.4">
+      <c r="L275" s="255"/>
+      <c r="M275" s="255"/>
+      <c r="N275" s="255"/>
+      <c r="O275" s="255"/>
+      <c r="P275" s="255"/>
+      <c r="Q275" s="255"/>
+      <c r="R275" s="256"/>
+    </row>
+    <row r="276" spans="12:18" ht="23.4">
+      <c r="L276" s="255"/>
+      <c r="M276" s="255"/>
+      <c r="N276" s="255"/>
+      <c r="O276" s="255"/>
+      <c r="P276" s="255"/>
+      <c r="Q276" s="255"/>
+      <c r="R276" s="256"/>
+    </row>
+    <row r="277" spans="12:18" ht="23.4">
+      <c r="L277" s="255"/>
+      <c r="M277" s="255"/>
+      <c r="N277" s="255"/>
+      <c r="O277" s="255"/>
+      <c r="P277" s="255"/>
+      <c r="Q277" s="255"/>
+      <c r="R277" s="256"/>
+    </row>
+    <row r="278" spans="12:18" ht="23.4">
+      <c r="L278" s="255"/>
+      <c r="M278" s="255"/>
+      <c r="N278" s="255"/>
+      <c r="O278" s="255"/>
+      <c r="P278" s="255"/>
+      <c r="Q278" s="255"/>
+      <c r="R278" s="256"/>
+    </row>
+    <row r="279" spans="12:18" ht="23.4">
+      <c r="L279" s="255"/>
+      <c r="M279" s="255"/>
+      <c r="N279" s="255"/>
+      <c r="O279" s="255"/>
+      <c r="P279" s="255"/>
+      <c r="Q279" s="255"/>
+      <c r="R279" s="256"/>
+    </row>
+    <row r="280" spans="12:18" ht="23.4">
+      <c r="L280" s="255"/>
+      <c r="M280" s="255"/>
+      <c r="N280" s="255"/>
+      <c r="O280" s="255"/>
+      <c r="P280" s="255"/>
+      <c r="Q280" s="255"/>
+      <c r="R280" s="256"/>
+    </row>
+    <row r="281" spans="12:18" ht="23.4">
+      <c r="L281" s="255"/>
+      <c r="M281" s="255"/>
+      <c r="N281" s="255"/>
+      <c r="O281" s="255"/>
+      <c r="P281" s="255"/>
+      <c r="Q281" s="255"/>
+      <c r="R281" s="256"/>
+    </row>
+    <row r="282" spans="12:18" ht="23.4">
+      <c r="L282" s="255"/>
+      <c r="M282" s="255"/>
+      <c r="N282" s="255"/>
+      <c r="O282" s="255"/>
+      <c r="P282" s="255"/>
+      <c r="Q282" s="255"/>
+      <c r="R282" s="256"/>
+    </row>
+    <row r="283" spans="12:18" ht="23.4">
+      <c r="L283" s="255"/>
+      <c r="M283" s="255"/>
+      <c r="N283" s="255"/>
+      <c r="O283" s="255"/>
+      <c r="P283" s="255"/>
+      <c r="Q283" s="255"/>
+      <c r="R283" s="256"/>
+    </row>
+    <row r="284" spans="12:18" ht="23.4">
+      <c r="L284" s="255"/>
+      <c r="M284" s="255"/>
+      <c r="N284" s="255"/>
+      <c r="O284" s="255"/>
+      <c r="P284" s="255"/>
+      <c r="Q284" s="255"/>
+      <c r="R284" s="256"/>
+    </row>
+    <row r="285" spans="12:18" ht="23.4">
+      <c r="L285" s="255"/>
+      <c r="M285" s="255"/>
+      <c r="N285" s="255"/>
+      <c r="O285" s="255"/>
+      <c r="P285" s="255"/>
+      <c r="Q285" s="255"/>
+      <c r="R285" s="256"/>
+    </row>
+    <row r="286" spans="12:18" ht="23.4">
+      <c r="L286" s="255"/>
+      <c r="M286" s="255"/>
+      <c r="N286" s="255"/>
+      <c r="O286" s="255"/>
+      <c r="P286" s="255"/>
+      <c r="Q286" s="255"/>
+      <c r="R286" s="256"/>
+    </row>
+    <row r="287" spans="12:18" ht="23.4">
+      <c r="L287" s="255"/>
+      <c r="M287" s="255"/>
+      <c r="N287" s="255"/>
+      <c r="O287" s="255"/>
+      <c r="P287" s="255"/>
+      <c r="Q287" s="255"/>
+      <c r="R287" s="256"/>
+    </row>
+    <row r="288" spans="12:18" ht="23.4">
+      <c r="L288" s="255"/>
+      <c r="M288" s="255"/>
+      <c r="N288" s="255"/>
+      <c r="O288" s="255"/>
+      <c r="P288" s="255"/>
+      <c r="Q288" s="255"/>
+      <c r="R288" s="256"/>
+    </row>
+    <row r="289" spans="12:18" ht="23.4">
+      <c r="L289" s="255"/>
+      <c r="M289" s="255"/>
+      <c r="N289" s="255"/>
+      <c r="O289" s="255"/>
+      <c r="P289" s="255"/>
+      <c r="Q289" s="255"/>
+      <c r="R289" s="256"/>
+    </row>
+    <row r="290" spans="12:18" ht="23.4">
+      <c r="L290" s="255"/>
+      <c r="M290" s="255"/>
+      <c r="N290" s="255"/>
+      <c r="O290" s="255"/>
+      <c r="P290" s="255"/>
+      <c r="Q290" s="255"/>
+      <c r="R290" s="256"/>
+    </row>
+    <row r="291" spans="12:18" ht="23.4">
+      <c r="L291" s="255"/>
+      <c r="M291" s="255"/>
+      <c r="N291" s="255"/>
+      <c r="O291" s="255"/>
+      <c r="P291" s="255"/>
+      <c r="Q291" s="255"/>
+      <c r="R291" s="256"/>
+    </row>
+    <row r="292" spans="12:18" ht="23.4">
+      <c r="L292" s="255"/>
+      <c r="M292" s="255"/>
+      <c r="N292" s="255"/>
+      <c r="O292" s="255"/>
+      <c r="P292" s="255"/>
+      <c r="Q292" s="255"/>
+      <c r="R292" s="256"/>
+    </row>
+    <row r="293" spans="12:18" ht="23.4">
+      <c r="L293" s="255"/>
+      <c r="M293" s="255"/>
+      <c r="N293" s="255"/>
+      <c r="O293" s="255"/>
+      <c r="P293" s="255"/>
+      <c r="Q293" s="255"/>
+      <c r="R293" s="256"/>
+    </row>
+    <row r="294" spans="12:18" ht="23.4">
+      <c r="L294" s="255"/>
+      <c r="M294" s="255"/>
+      <c r="N294" s="255"/>
+      <c r="O294" s="255"/>
+      <c r="P294" s="255"/>
+      <c r="Q294" s="255"/>
+      <c r="R294" s="256"/>
+    </row>
+    <row r="295" spans="12:18" ht="23.4">
+      <c r="L295" s="255"/>
+      <c r="M295" s="255"/>
+      <c r="N295" s="255"/>
+      <c r="O295" s="255"/>
+      <c r="P295" s="255"/>
+      <c r="Q295" s="255"/>
+      <c r="R295" s="256"/>
+    </row>
+    <row r="296" spans="12:18" ht="23.4">
+      <c r="L296" s="255"/>
+      <c r="M296" s="255"/>
+      <c r="N296" s="255"/>
+      <c r="O296" s="255"/>
+      <c r="P296" s="255"/>
+      <c r="Q296" s="255"/>
+      <c r="R296" s="256"/>
+    </row>
+    <row r="297" spans="12:18" ht="23.4">
+      <c r="L297" s="255"/>
+      <c r="M297" s="255"/>
+      <c r="N297" s="255"/>
+      <c r="O297" s="255"/>
+      <c r="P297" s="255"/>
+      <c r="Q297" s="255"/>
+      <c r="R297" s="256"/>
+    </row>
+    <row r="298" spans="12:18" ht="23.4">
+      <c r="L298" s="255"/>
+      <c r="M298" s="255"/>
+      <c r="N298" s="255"/>
+      <c r="O298" s="255"/>
+      <c r="P298" s="255"/>
+      <c r="Q298" s="255"/>
+      <c r="R298" s="256"/>
+    </row>
+    <row r="299" spans="12:18" ht="23.4">
+      <c r="L299" s="255"/>
+      <c r="M299" s="255"/>
+      <c r="N299" s="255"/>
+      <c r="O299" s="255"/>
+      <c r="P299" s="255"/>
+      <c r="Q299" s="255"/>
+      <c r="R299" s="256"/>
+    </row>
+    <row r="300" spans="12:18" ht="23.4">
+      <c r="L300" s="255"/>
+      <c r="M300" s="255"/>
+      <c r="N300" s="255"/>
+      <c r="O300" s="255"/>
+      <c r="P300" s="255"/>
+      <c r="Q300" s="255"/>
+      <c r="R300" s="256"/>
+    </row>
+    <row r="301" spans="12:18" ht="23.4">
+      <c r="L301" s="255"/>
+      <c r="M301" s="255"/>
+      <c r="N301" s="255"/>
+      <c r="O301" s="255"/>
+      <c r="P301" s="255"/>
+      <c r="Q301" s="255"/>
+      <c r="R301" s="256"/>
+    </row>
+    <row r="302" spans="12:18" ht="23.4">
+      <c r="L302" s="255"/>
+      <c r="M302" s="255"/>
+      <c r="N302" s="255"/>
+      <c r="O302" s="255"/>
+      <c r="P302" s="255"/>
+      <c r="Q302" s="255"/>
+      <c r="R302" s="256"/>
+    </row>
+    <row r="303" spans="12:18" ht="23.4">
+      <c r="L303" s="255"/>
+      <c r="M303" s="255"/>
+      <c r="N303" s="255"/>
+      <c r="O303" s="255"/>
+      <c r="P303" s="255"/>
+      <c r="Q303" s="255"/>
+      <c r="R303" s="256"/>
+    </row>
+    <row r="304" spans="12:18" ht="23.4">
+      <c r="L304" s="255"/>
+      <c r="M304" s="255"/>
+      <c r="N304" s="255"/>
+      <c r="O304" s="255"/>
+      <c r="P304" s="255"/>
+      <c r="Q304" s="255"/>
+      <c r="R304" s="256"/>
+    </row>
+    <row r="305" spans="12:18" ht="23.4">
+      <c r="L305" s="255"/>
+      <c r="M305" s="255"/>
+      <c r="N305" s="255"/>
+      <c r="O305" s="255"/>
+      <c r="P305" s="255"/>
+      <c r="Q305" s="255"/>
+      <c r="R305" s="256"/>
+    </row>
+    <row r="306" spans="12:18" ht="23.4">
+      <c r="L306" s="255"/>
+      <c r="M306" s="255"/>
+      <c r="N306" s="255"/>
+      <c r="O306" s="255"/>
+      <c r="P306" s="255"/>
+      <c r="Q306" s="255"/>
+      <c r="R306" s="256"/>
+    </row>
+    <row r="307" spans="12:18" ht="23.4">
+      <c r="L307" s="255"/>
+      <c r="M307" s="255"/>
+      <c r="N307" s="255"/>
+      <c r="O307" s="255"/>
+      <c r="P307" s="255"/>
+      <c r="Q307" s="255"/>
+      <c r="R307" s="256"/>
+    </row>
+    <row r="308" spans="12:18" ht="23.4">
+      <c r="L308" s="255"/>
+      <c r="M308" s="255"/>
+      <c r="N308" s="255"/>
+      <c r="O308" s="255"/>
+      <c r="P308" s="255"/>
+      <c r="Q308" s="255"/>
+      <c r="R308" s="256"/>
+    </row>
+    <row r="309" spans="12:18" ht="23.4">
+      <c r="L309" s="255"/>
+      <c r="M309" s="255"/>
+      <c r="N309" s="255"/>
+      <c r="O309" s="255"/>
+      <c r="P309" s="255"/>
+      <c r="Q309" s="255"/>
+      <c r="R309" s="256"/>
+    </row>
+    <row r="310" spans="12:18" ht="23.4">
+      <c r="L310" s="255"/>
+      <c r="M310" s="255"/>
+      <c r="N310" s="255"/>
+      <c r="O310" s="255"/>
+      <c r="P310" s="255"/>
+      <c r="Q310" s="255"/>
+      <c r="R310" s="256"/>
+    </row>
+    <row r="311" spans="12:18" ht="23.4">
+      <c r="L311" s="255"/>
+      <c r="M311" s="255"/>
+      <c r="N311" s="255"/>
+      <c r="O311" s="255"/>
+      <c r="P311" s="255"/>
+      <c r="Q311" s="255"/>
+      <c r="R311" s="256"/>
+    </row>
+    <row r="312" spans="12:18" ht="23.4">
+      <c r="L312" s="255"/>
+      <c r="M312" s="255"/>
+      <c r="N312" s="255"/>
+      <c r="O312" s="255"/>
+      <c r="P312" s="255"/>
+      <c r="Q312" s="255"/>
+      <c r="R312" s="256"/>
+    </row>
+    <row r="313" spans="12:18" ht="23.4">
+      <c r="L313" s="255"/>
+      <c r="M313" s="255"/>
+      <c r="N313" s="255"/>
+      <c r="O313" s="255"/>
+      <c r="P313" s="255"/>
+      <c r="Q313" s="255"/>
+      <c r="R313" s="256"/>
+    </row>
+    <row r="314" spans="12:18" ht="23.4">
+      <c r="L314" s="255"/>
+      <c r="M314" s="255"/>
+      <c r="N314" s="255"/>
+      <c r="O314" s="255"/>
+      <c r="P314" s="255"/>
+      <c r="Q314" s="255"/>
+      <c r="R314" s="256"/>
+    </row>
+    <row r="315" spans="12:18" ht="23.4">
+      <c r="L315" s="255"/>
+      <c r="M315" s="255"/>
+      <c r="N315" s="255"/>
+      <c r="O315" s="255"/>
+      <c r="P315" s="255"/>
+      <c r="Q315" s="255"/>
+      <c r="R315" s="256"/>
+    </row>
+    <row r="316" spans="12:18" ht="23.4">
+      <c r="L316" s="255"/>
+      <c r="M316" s="255"/>
+      <c r="N316" s="255"/>
+      <c r="O316" s="255"/>
+      <c r="P316" s="255"/>
+      <c r="Q316" s="255"/>
+      <c r="R316" s="256"/>
+    </row>
+    <row r="317" spans="12:18" ht="23.4">
+      <c r="L317" s="255"/>
+      <c r="M317" s="255"/>
+      <c r="N317" s="255"/>
+      <c r="O317" s="255"/>
+      <c r="P317" s="255"/>
+      <c r="Q317" s="255"/>
+      <c r="R317" s="256"/>
+    </row>
+    <row r="318" spans="12:18" ht="23.4">
+      <c r="L318" s="255"/>
+      <c r="M318" s="255"/>
+      <c r="N318" s="255"/>
+      <c r="O318" s="255"/>
+      <c r="P318" s="255"/>
+      <c r="Q318" s="255"/>
+      <c r="R318" s="256"/>
+    </row>
+    <row r="319" spans="12:18" ht="23.4">
+      <c r="L319" s="255"/>
+      <c r="M319" s="255"/>
+      <c r="N319" s="255"/>
+      <c r="O319" s="255"/>
+      <c r="P319" s="255"/>
+      <c r="Q319" s="255"/>
+      <c r="R319" s="256"/>
+    </row>
+    <row r="320" spans="12:18" ht="23.4">
+      <c r="L320" s="255"/>
+      <c r="M320" s="255"/>
+      <c r="N320" s="255"/>
+      <c r="O320" s="255"/>
+      <c r="P320" s="255"/>
+      <c r="Q320" s="255"/>
+      <c r="R320" s="256"/>
+    </row>
+    <row r="321" spans="12:18" ht="23.4">
+      <c r="L321" s="255"/>
+      <c r="M321" s="255"/>
+      <c r="N321" s="255"/>
+      <c r="O321" s="255"/>
+      <c r="P321" s="255"/>
+      <c r="Q321" s="255"/>
+      <c r="R321" s="256"/>
+    </row>
+    <row r="322" spans="12:18" ht="23.4">
+      <c r="L322" s="255"/>
+      <c r="M322" s="255"/>
+      <c r="N322" s="255"/>
+      <c r="O322" s="255"/>
+      <c r="P322" s="255"/>
+      <c r="Q322" s="255"/>
+      <c r="R322" s="256"/>
+    </row>
+    <row r="323" spans="12:18" ht="23.4">
+      <c r="L323" s="255"/>
+      <c r="M323" s="255"/>
+      <c r="N323" s="255"/>
+      <c r="O323" s="255"/>
+      <c r="P323" s="255"/>
+      <c r="Q323" s="255"/>
+      <c r="R323" s="256"/>
+    </row>
+    <row r="324" spans="12:18" ht="23.4">
+      <c r="L324" s="255"/>
+      <c r="M324" s="255"/>
+      <c r="N324" s="255"/>
+      <c r="O324" s="255"/>
+      <c r="P324" s="255"/>
+      <c r="Q324" s="255"/>
+      <c r="R324" s="256"/>
+    </row>
+    <row r="325" spans="12:18" ht="23.4">
+      <c r="L325" s="255"/>
+      <c r="M325" s="255"/>
+      <c r="N325" s="255"/>
+      <c r="O325" s="255"/>
+      <c r="P325" s="255"/>
+      <c r="Q325" s="255"/>
+      <c r="R325" s="256"/>
+    </row>
+    <row r="326" spans="12:18" ht="23.4">
+      <c r="L326" s="255"/>
+      <c r="M326" s="255"/>
+      <c r="N326" s="255"/>
+      <c r="O326" s="255"/>
+      <c r="P326" s="255"/>
+      <c r="Q326" s="255"/>
+      <c r="R326" s="256"/>
+    </row>
+    <row r="327" spans="12:18" ht="23.4">
+      <c r="L327" s="255"/>
+      <c r="M327" s="255"/>
+      <c r="N327" s="255"/>
+      <c r="O327" s="255"/>
+      <c r="P327" s="255"/>
+      <c r="Q327" s="255"/>
+      <c r="R327" s="256"/>
+    </row>
+    <row r="328" spans="12:18" ht="23.4">
+      <c r="L328" s="255"/>
+      <c r="M328" s="255"/>
+      <c r="N328" s="255"/>
+      <c r="O328" s="255"/>
+      <c r="P328" s="255"/>
+      <c r="Q328" s="255"/>
+      <c r="R328" s="256"/>
+    </row>
+    <row r="329" spans="12:18" ht="23.4">
+      <c r="L329" s="255"/>
+      <c r="M329" s="255"/>
+      <c r="N329" s="255"/>
+      <c r="O329" s="255"/>
+      <c r="P329" s="255"/>
+      <c r="Q329" s="255"/>
+      <c r="R329" s="256"/>
+    </row>
+    <row r="330" spans="12:18" ht="23.4">
+      <c r="L330" s="255"/>
+      <c r="M330" s="255"/>
+      <c r="N330" s="255"/>
+      <c r="O330" s="255"/>
+      <c r="P330" s="255"/>
+      <c r="Q330" s="255"/>
+      <c r="R330" s="256"/>
+    </row>
+    <row r="331" spans="12:18" ht="23.4">
+      <c r="L331" s="255"/>
+      <c r="M331" s="255"/>
+      <c r="N331" s="255"/>
+      <c r="O331" s="255"/>
+      <c r="P331" s="255"/>
+      <c r="Q331" s="255"/>
+      <c r="R331" s="256"/>
+    </row>
+    <row r="332" spans="12:18" ht="23.4">
+      <c r="L332" s="255"/>
+      <c r="M332" s="255"/>
+      <c r="N332" s="255"/>
+      <c r="O332" s="255"/>
+      <c r="P332" s="255"/>
+      <c r="Q332" s="255"/>
+      <c r="R332" s="256"/>
+    </row>
+    <row r="333" spans="12:18" ht="23.4">
+      <c r="L333" s="255"/>
+      <c r="M333" s="255"/>
+      <c r="N333" s="255"/>
+      <c r="O333" s="255"/>
+      <c r="P333" s="255"/>
+      <c r="Q333" s="255"/>
+      <c r="R333" s="256"/>
+    </row>
+    <row r="334" spans="12:18" ht="23.4">
+      <c r="L334" s="255"/>
+      <c r="M334" s="255"/>
+      <c r="N334" s="255"/>
+      <c r="O334" s="255"/>
+      <c r="P334" s="255"/>
+      <c r="Q334" s="255"/>
+      <c r="R334" s="256"/>
+    </row>
+    <row r="335" spans="12:18" ht="23.4">
+      <c r="L335" s="255"/>
+      <c r="M335" s="255"/>
+      <c r="N335" s="255"/>
+      <c r="O335" s="255"/>
+      <c r="P335" s="255"/>
+      <c r="Q335" s="255"/>
+      <c r="R335" s="256"/>
+    </row>
+    <row r="336" spans="12:18" ht="23.4">
+      <c r="L336" s="255"/>
+      <c r="M336" s="255"/>
+      <c r="N336" s="255"/>
+      <c r="O336" s="255"/>
+      <c r="P336" s="255"/>
+      <c r="Q336" s="255"/>
+      <c r="R336" s="256"/>
+    </row>
+    <row r="337" spans="12:18" ht="23.4">
+      <c r="L337" s="255"/>
+      <c r="M337" s="255"/>
+      <c r="N337" s="255"/>
+      <c r="O337" s="255"/>
+      <c r="P337" s="255"/>
+      <c r="Q337" s="255"/>
+      <c r="R337" s="256"/>
+    </row>
+    <row r="338" spans="12:18" ht="23.4">
+      <c r="L338" s="255"/>
+      <c r="M338" s="255"/>
+      <c r="N338" s="255"/>
+      <c r="O338" s="255"/>
+      <c r="P338" s="255"/>
+      <c r="Q338" s="255"/>
+      <c r="R338" s="256"/>
+    </row>
+    <row r="339" spans="12:18" ht="23.4">
+      <c r="L339" s="255"/>
+      <c r="M339" s="255"/>
+      <c r="N339" s="255"/>
+      <c r="O339" s="255"/>
+      <c r="P339" s="255"/>
+      <c r="Q339" s="255"/>
+      <c r="R339" s="256"/>
+    </row>
+    <row r="340" spans="12:18" ht="23.4">
+      <c r="L340" s="255"/>
+      <c r="M340" s="255"/>
+      <c r="N340" s="255"/>
+      <c r="O340" s="255"/>
+      <c r="P340" s="255"/>
+      <c r="Q340" s="255"/>
+      <c r="R340" s="256"/>
+    </row>
+    <row r="341" spans="12:18" ht="23.4">
+      <c r="L341" s="255"/>
+      <c r="M341" s="255"/>
+      <c r="N341" s="255"/>
+      <c r="O341" s="255"/>
+      <c r="P341" s="255"/>
+      <c r="Q341" s="255"/>
+      <c r="R341" s="256"/>
+    </row>
+    <row r="342" spans="12:18" ht="23.4">
+      <c r="L342" s="255"/>
+      <c r="M342" s="255"/>
+      <c r="N342" s="255"/>
+      <c r="O342" s="255"/>
+      <c r="P342" s="255"/>
+      <c r="Q342" s="255"/>
+      <c r="R342" s="256"/>
+    </row>
+    <row r="343" spans="12:18" ht="23.4">
+      <c r="L343" s="255"/>
+      <c r="M343" s="255"/>
+      <c r="N343" s="255"/>
+      <c r="O343" s="255"/>
+      <c r="P343" s="255"/>
+      <c r="Q343" s="255"/>
+      <c r="R343" s="256"/>
+    </row>
+    <row r="344" spans="12:18" ht="23.4">
+      <c r="L344" s="255"/>
+      <c r="M344" s="255"/>
+      <c r="N344" s="255"/>
+      <c r="O344" s="255"/>
+      <c r="P344" s="255"/>
+      <c r="Q344" s="255"/>
+      <c r="R344" s="256"/>
+    </row>
+    <row r="345" spans="12:18" ht="23.4">
+      <c r="L345" s="255"/>
+      <c r="M345" s="255"/>
+      <c r="N345" s="255"/>
+      <c r="O345" s="255"/>
+      <c r="P345" s="255"/>
+      <c r="Q345" s="255"/>
+      <c r="R345" s="256"/>
+    </row>
+    <row r="346" spans="12:18" ht="23.4">
+      <c r="L346" s="255"/>
+      <c r="M346" s="255"/>
+      <c r="N346" s="255"/>
+      <c r="O346" s="255"/>
+      <c r="P346" s="255"/>
+      <c r="Q346" s="255"/>
+      <c r="R346" s="256"/>
+    </row>
+    <row r="347" spans="12:18" ht="23.4">
+      <c r="L347" s="255"/>
+      <c r="M347" s="255"/>
+      <c r="N347" s="255"/>
+      <c r="O347" s="255"/>
+      <c r="P347" s="255"/>
+      <c r="Q347" s="255"/>
+      <c r="R347" s="256"/>
+    </row>
+    <row r="348" spans="12:18" ht="23.4">
+      <c r="L348" s="255"/>
+      <c r="M348" s="255"/>
+      <c r="N348" s="255"/>
+      <c r="O348" s="255"/>
+      <c r="P348" s="255"/>
+      <c r="Q348" s="255"/>
+      <c r="R348" s="256"/>
+    </row>
+    <row r="349" spans="12:18" ht="23.4">
+      <c r="L349" s="255"/>
+      <c r="M349" s="255"/>
+      <c r="N349" s="255"/>
+      <c r="O349" s="255"/>
+      <c r="P349" s="255"/>
+      <c r="Q349" s="255"/>
+      <c r="R349" s="256"/>
+    </row>
+    <row r="350" spans="12:18" ht="23.4">
+      <c r="L350" s="255"/>
+      <c r="M350" s="255"/>
+      <c r="N350" s="255"/>
+      <c r="O350" s="255"/>
+      <c r="P350" s="255"/>
+      <c r="Q350" s="255"/>
+      <c r="R350" s="256"/>
+    </row>
+    <row r="351" spans="12:18" ht="23.4">
+      <c r="L351" s="255"/>
+      <c r="M351" s="255"/>
+      <c r="N351" s="255"/>
+      <c r="O351" s="255"/>
+      <c r="P351" s="255"/>
+      <c r="Q351" s="255"/>
+      <c r="R351" s="256"/>
+    </row>
+    <row r="352" spans="12:18" ht="23.4">
+      <c r="L352" s="255"/>
+      <c r="M352" s="255"/>
+      <c r="N352" s="255"/>
+      <c r="O352" s="255"/>
+      <c r="P352" s="255"/>
+      <c r="Q352" s="255"/>
+      <c r="R352" s="256"/>
+    </row>
+    <row r="353" spans="12:18" ht="23.4">
+      <c r="L353" s="255"/>
+      <c r="M353" s="255"/>
+      <c r="N353" s="255"/>
+      <c r="O353" s="255"/>
+      <c r="P353" s="255"/>
+      <c r="Q353" s="255"/>
+      <c r="R353" s="256"/>
+    </row>
+    <row r="354" spans="12:18" ht="23.4">
+      <c r="L354" s="255"/>
+      <c r="M354" s="255"/>
+      <c r="N354" s="255"/>
+      <c r="O354" s="255"/>
+      <c r="P354" s="255"/>
+      <c r="Q354" s="255"/>
+      <c r="R354" s="256"/>
+    </row>
+    <row r="355" spans="12:18" ht="23.4">
+      <c r="L355" s="255"/>
+      <c r="M355" s="255"/>
+      <c r="N355" s="255"/>
+      <c r="O355" s="255"/>
+      <c r="P355" s="255"/>
+      <c r="Q355" s="255"/>
+      <c r="R355" s="256"/>
+    </row>
+    <row r="356" spans="12:18" ht="23.4">
+      <c r="L356" s="255"/>
+      <c r="M356" s="255"/>
+      <c r="N356" s="255"/>
+      <c r="O356" s="255"/>
+      <c r="P356" s="255"/>
+      <c r="Q356" s="255"/>
+      <c r="R356" s="256"/>
+    </row>
+    <row r="357" spans="12:18" ht="23.4">
+      <c r="L357" s="255"/>
+      <c r="M357" s="255"/>
+      <c r="N357" s="255"/>
+      <c r="O357" s="255"/>
+      <c r="P357" s="255"/>
+      <c r="Q357" s="255"/>
+      <c r="R357" s="256"/>
+    </row>
+    <row r="358" spans="12:18" ht="23.4">
+      <c r="L358" s="255"/>
+      <c r="M358" s="255"/>
+      <c r="N358" s="255"/>
+      <c r="O358" s="255"/>
+      <c r="P358" s="255"/>
+      <c r="Q358" s="255"/>
+      <c r="R358" s="256"/>
     </row>
   </sheetData>
   <autoFilter ref="A3:J26"/>
-  <mergeCells count="1">
-    <mergeCell ref="A1:J1"/>
+  <mergeCells count="2">
+    <mergeCell ref="A1:R1"/>
+    <mergeCell ref="A2:R2"/>
   </mergeCells>
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.24000000000000002" right="0.24000000000000002" top="0.75000000000000011" bottom="0.75000000000000011" header="0.31" footer="0.31"/>
@@ -6254,24 +9348,24 @@
   <sheetData>
     <row r="1" spans="1:17" ht="16.2" thickBot="1">
       <c r="A1" s="2"/>
-      <c r="B1" s="259" t="s">
+      <c r="B1" s="250" t="s">
         <v>465</v>
       </c>
-      <c r="C1" s="260"/>
-      <c r="D1" s="260"/>
-      <c r="E1" s="260"/>
-      <c r="F1" s="260"/>
-      <c r="G1" s="260"/>
-      <c r="H1" s="260"/>
-      <c r="I1" s="260"/>
-      <c r="J1" s="260"/>
-      <c r="K1" s="260"/>
-      <c r="L1" s="260"/>
-      <c r="M1" s="260"/>
-      <c r="N1" s="260"/>
-      <c r="O1" s="260"/>
-      <c r="P1" s="260"/>
-      <c r="Q1" s="261"/>
+      <c r="C1" s="251"/>
+      <c r="D1" s="251"/>
+      <c r="E1" s="251"/>
+      <c r="F1" s="251"/>
+      <c r="G1" s="251"/>
+      <c r="H1" s="251"/>
+      <c r="I1" s="251"/>
+      <c r="J1" s="251"/>
+      <c r="K1" s="251"/>
+      <c r="L1" s="251"/>
+      <c r="M1" s="251"/>
+      <c r="N1" s="251"/>
+      <c r="O1" s="251"/>
+      <c r="P1" s="251"/>
+      <c r="Q1" s="252"/>
     </row>
     <row r="2" spans="1:17" ht="20.399999999999999" thickBot="1">
       <c r="A2" s="2"/>

</xml_diff>